<commit_message>
YP-CORE_2_scores: finally fixed the error trapping and changed status from work in progress to released for use. Updated csv, ods, xlsx and Rda files to replace NA with blank entries.
</commit_message>
<xml_diff>
--- a/docs/YP-CORE/YPwide2.xlsx
+++ b/docs/YP-CORE/YPwide2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Current_share\Current_Data\MyR\shiny.psyctc.org\docs\YP-CORE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F5A59C-2749-4666-A427-D067A33FFDAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DE1A440-8D7A-40F6-B6E1-AF153E0E5532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="19935" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14535" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="YPwide2" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="28">
   <si>
     <t>RespondentID</t>
   </si>
@@ -1027,9 +1027,6 @@
       <c r="H15">
         <v>31.5</v>
       </c>
-      <c r="I15" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J15" s="1">
         <v>44434</v>
       </c>
@@ -1077,9 +1074,6 @@
       <c r="H16">
         <v>31.5</v>
       </c>
-      <c r="I16" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J16" s="1">
         <v>44204</v>
       </c>
@@ -1127,9 +1121,6 @@
       <c r="H17" t="s">
         <v>17</v>
       </c>
-      <c r="I17" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J17" s="1">
         <v>43858</v>
       </c>
@@ -1176,9 +1167,6 @@
       </c>
       <c r="H18">
         <v>12</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="J18" s="1">
         <v>44413</v>
@@ -1227,9 +1215,6 @@
       <c r="H19">
         <v>31.5</v>
       </c>
-      <c r="I19" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J19" s="1">
         <v>44084</v>
       </c>
@@ -1277,9 +1262,6 @@
       <c r="H20">
         <v>17.899999999999999</v>
       </c>
-      <c r="I20" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J20" s="1">
         <v>44133</v>
       </c>
@@ -1327,9 +1309,6 @@
       <c r="H21">
         <v>17.5</v>
       </c>
-      <c r="I21" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J21" s="1">
         <v>44470</v>
       </c>
@@ -1377,9 +1356,6 @@
       <c r="H22">
         <v>20.9</v>
       </c>
-      <c r="I22" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J22" s="1">
         <v>44040</v>
       </c>
@@ -1427,9 +1403,6 @@
       <c r="H23">
         <v>11</v>
       </c>
-      <c r="I23" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J23" s="1">
         <v>44168</v>
       </c>
@@ -1477,9 +1450,6 @@
       <c r="H24">
         <v>23.8</v>
       </c>
-      <c r="I24" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J24" s="1">
         <v>44069</v>
       </c>
@@ -1527,9 +1497,6 @@
       <c r="H25">
         <v>22.3</v>
       </c>
-      <c r="I25" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J25" s="1">
         <v>44418</v>
       </c>
@@ -1577,9 +1544,6 @@
       <c r="H26">
         <v>10.8</v>
       </c>
-      <c r="I26" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J26" s="1">
         <v>44194</v>
       </c>
@@ -1627,9 +1591,6 @@
       <c r="H27">
         <v>10.5</v>
       </c>
-      <c r="I27" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J27" s="1">
         <v>44020</v>
       </c>
@@ -1677,9 +1638,6 @@
       <c r="H28">
         <v>19.899999999999999</v>
       </c>
-      <c r="I28" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J28" s="1">
         <v>43887</v>
       </c>
@@ -1727,9 +1685,6 @@
       <c r="H29">
         <v>9.1999999999999993</v>
       </c>
-      <c r="I29" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J29" s="1">
         <v>44159</v>
       </c>
@@ -1777,9 +1732,6 @@
       <c r="H30">
         <v>27.4</v>
       </c>
-      <c r="I30" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J30" s="1">
         <v>44244</v>
       </c>
@@ -1827,9 +1779,6 @@
       <c r="H31">
         <v>14.4</v>
       </c>
-      <c r="I31" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J31" s="1">
         <v>44236</v>
       </c>
@@ -1877,9 +1826,6 @@
       <c r="H32">
         <v>23.8</v>
       </c>
-      <c r="I32" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J32" s="1">
         <v>44047</v>
       </c>
@@ -1927,9 +1873,6 @@
       <c r="H33">
         <v>13.1</v>
       </c>
-      <c r="I33" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J33" s="1">
         <v>44124</v>
       </c>
@@ -1977,9 +1920,6 @@
       <c r="H34">
         <v>17.3</v>
       </c>
-      <c r="I34" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J34" s="1">
         <v>43935</v>
       </c>
@@ -2027,9 +1967,6 @@
       <c r="H35">
         <v>17.3</v>
       </c>
-      <c r="I35" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J35" s="1">
         <v>44127</v>
       </c>
@@ -2077,9 +2014,6 @@
       <c r="H36">
         <v>20.399999999999999</v>
       </c>
-      <c r="I36" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J36" s="1">
         <v>43893</v>
       </c>
@@ -2127,9 +2061,6 @@
       <c r="H37">
         <v>14.4</v>
       </c>
-      <c r="I37" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J37" s="1">
         <v>44238</v>
       </c>
@@ -2177,9 +2108,6 @@
       <c r="H38">
         <v>18.5</v>
       </c>
-      <c r="I38" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J38" s="1">
         <v>44166</v>
       </c>
@@ -2227,9 +2155,6 @@
       <c r="H39">
         <v>19</v>
       </c>
-      <c r="I39" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J39" s="1">
         <v>44125</v>
       </c>
@@ -2277,9 +2202,6 @@
       <c r="H40">
         <v>23.4</v>
       </c>
-      <c r="I40" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J40" s="1">
         <v>44440</v>
       </c>
@@ -2327,9 +2249,6 @@
       <c r="H41">
         <v>16.2</v>
       </c>
-      <c r="I41" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J41" s="1">
         <v>43852</v>
       </c>
@@ -2377,9 +2296,6 @@
       <c r="H42">
         <v>15.3</v>
       </c>
-      <c r="I42" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J42" s="1">
         <v>44209</v>
       </c>
@@ -2427,9 +2343,6 @@
       <c r="H43">
         <v>23.5</v>
       </c>
-      <c r="I43" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J43" s="1">
         <v>44287</v>
       </c>
@@ -2477,9 +2390,6 @@
       <c r="H44">
         <v>18.100000000000001</v>
       </c>
-      <c r="I44" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J44" s="1">
         <v>44125</v>
       </c>
@@ -2527,9 +2437,6 @@
       <c r="H45">
         <v>20.8</v>
       </c>
-      <c r="I45" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J45" s="1">
         <v>44442</v>
       </c>
@@ -2577,9 +2484,6 @@
       <c r="H46">
         <v>6.8</v>
       </c>
-      <c r="I46" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J46" s="1">
         <v>44251</v>
       </c>
@@ -2627,9 +2531,6 @@
       <c r="H47">
         <v>10.1</v>
       </c>
-      <c r="I47" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J47" s="1">
         <v>44469</v>
       </c>
@@ -2674,9 +2575,6 @@
       <c r="H48">
         <v>24.4</v>
       </c>
-      <c r="I48" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J48" s="1">
         <v>43846</v>
       </c>
@@ -2724,9 +2622,6 @@
       <c r="H49">
         <v>16.7</v>
       </c>
-      <c r="I49" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J49" s="1">
         <v>44182</v>
       </c>
@@ -2774,9 +2669,6 @@
       <c r="H50">
         <v>12.6</v>
       </c>
-      <c r="I50" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J50" s="1">
         <v>44232</v>
       </c>
@@ -2824,9 +2716,6 @@
       <c r="H51">
         <v>6.5</v>
       </c>
-      <c r="I51" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J51" s="1">
         <v>44113</v>
       </c>
@@ -2874,9 +2763,6 @@
       <c r="H52">
         <v>7</v>
       </c>
-      <c r="I52" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J52" s="1">
         <v>44461</v>
       </c>
@@ -2924,9 +2810,6 @@
       <c r="H53">
         <v>15.1</v>
       </c>
-      <c r="I53" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J53" s="1">
         <v>44209</v>
       </c>
@@ -2974,9 +2857,6 @@
       <c r="H54">
         <v>26.8</v>
       </c>
-      <c r="I54" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J54" s="1">
         <v>44462</v>
       </c>
@@ -3024,9 +2904,6 @@
       <c r="H55">
         <v>15.9</v>
       </c>
-      <c r="I55" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J55" s="1">
         <v>44084</v>
       </c>
@@ -3074,9 +2951,6 @@
       <c r="H56">
         <v>13.5</v>
       </c>
-      <c r="I56" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J56" s="1">
         <v>44337</v>
       </c>
@@ -3124,9 +2998,6 @@
       <c r="H57">
         <v>15.3</v>
       </c>
-      <c r="I57" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J57" s="1">
         <v>44400</v>
       </c>
@@ -3174,9 +3045,6 @@
       <c r="H58">
         <v>16.899999999999999</v>
       </c>
-      <c r="I58" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J58" s="1">
         <v>44420</v>
       </c>
@@ -3224,9 +3092,6 @@
       <c r="H59">
         <v>12.2</v>
       </c>
-      <c r="I59" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J59" s="1">
         <v>44330</v>
       </c>
@@ -3274,9 +3139,6 @@
       <c r="H60">
         <v>6.7</v>
       </c>
-      <c r="I60" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J60" s="1">
         <v>43952</v>
       </c>
@@ -3324,9 +3186,6 @@
       <c r="H61">
         <v>26.5</v>
       </c>
-      <c r="I61" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J61" s="1">
         <v>44092</v>
       </c>
@@ -3374,9 +3233,6 @@
       <c r="H62">
         <v>23</v>
       </c>
-      <c r="I62" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J62" s="1">
         <v>43861</v>
       </c>
@@ -3424,9 +3280,6 @@
       <c r="H63">
         <v>18.5</v>
       </c>
-      <c r="I63" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J63" s="1">
         <v>43972</v>
       </c>
@@ -3474,9 +3327,6 @@
       <c r="H64">
         <v>10.5</v>
       </c>
-      <c r="I64" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J64" s="1">
         <v>44370</v>
       </c>
@@ -3524,9 +3374,6 @@
       <c r="H65">
         <v>23.4</v>
       </c>
-      <c r="I65" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J65" s="1">
         <v>44252</v>
       </c>
@@ -3574,9 +3421,6 @@
       <c r="H66">
         <v>27.6</v>
       </c>
-      <c r="I66" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J66" s="1">
         <v>43875</v>
       </c>
@@ -3624,9 +3468,6 @@
       <c r="H67">
         <v>16.600000000000001</v>
       </c>
-      <c r="I67" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J67" s="1">
         <v>44083</v>
       </c>
@@ -3674,9 +3515,6 @@
       <c r="H68">
         <v>24.3</v>
       </c>
-      <c r="I68" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J68" s="1">
         <v>43854</v>
       </c>
@@ -3724,9 +3562,6 @@
       <c r="H69">
         <v>5.6</v>
       </c>
-      <c r="I69" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J69" s="1">
         <v>44166</v>
       </c>
@@ -3774,9 +3609,6 @@
       <c r="H70">
         <v>22.8</v>
       </c>
-      <c r="I70" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J70" s="1">
         <v>44370</v>
       </c>
@@ -3824,9 +3656,6 @@
       <c r="H71">
         <v>21.7</v>
       </c>
-      <c r="I71" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J71" s="1">
         <v>44412</v>
       </c>
@@ -3874,9 +3703,6 @@
       <c r="H72">
         <v>8.1</v>
       </c>
-      <c r="I72" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J72" s="1">
         <v>44007</v>
       </c>
@@ -3924,9 +3750,6 @@
       <c r="H73">
         <v>14.1</v>
       </c>
-      <c r="I73" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J73" s="1">
         <v>44287</v>
       </c>
@@ -3974,9 +3797,6 @@
       <c r="H74">
         <v>19.100000000000001</v>
       </c>
-      <c r="I74" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J74" s="1">
         <v>44321</v>
       </c>
@@ -4024,9 +3844,6 @@
       <c r="H75">
         <v>9.1</v>
       </c>
-      <c r="I75" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J75" s="1">
         <v>44056</v>
       </c>
@@ -4074,9 +3891,6 @@
       <c r="H76">
         <v>21.5</v>
       </c>
-      <c r="I76" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J76" s="1">
         <v>44134</v>
       </c>
@@ -4124,9 +3938,6 @@
       <c r="H77">
         <v>22.4</v>
       </c>
-      <c r="I77" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J77" s="1">
         <v>43949</v>
       </c>
@@ -4174,9 +3985,6 @@
       <c r="H78">
         <v>26</v>
       </c>
-      <c r="I78" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J78" s="1">
         <v>44180</v>
       </c>
@@ -4224,9 +4032,6 @@
       <c r="H79">
         <v>23.9</v>
       </c>
-      <c r="I79" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J79" s="1">
         <v>43984</v>
       </c>
@@ -4274,9 +4079,6 @@
       <c r="H80">
         <v>30.1</v>
       </c>
-      <c r="I80" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J80" s="1">
         <v>43943</v>
       </c>
@@ -4324,9 +4126,6 @@
       <c r="H81">
         <v>18.7</v>
       </c>
-      <c r="I81" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J81" s="1">
         <v>44084</v>
       </c>
@@ -4374,9 +4173,6 @@
       <c r="H82">
         <v>22.3</v>
       </c>
-      <c r="I82" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J82" s="1">
         <v>44028</v>
       </c>
@@ -4424,9 +4220,6 @@
       <c r="H83">
         <v>17.7</v>
       </c>
-      <c r="I83" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J83" s="1">
         <v>44463</v>
       </c>
@@ -4474,9 +4267,6 @@
       <c r="H84">
         <v>24</v>
       </c>
-      <c r="I84" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J84" s="1">
         <v>44435</v>
       </c>
@@ -4524,9 +4314,6 @@
       <c r="H85">
         <v>23</v>
       </c>
-      <c r="I85" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J85" s="1">
         <v>44252</v>
       </c>
@@ -4574,9 +4361,6 @@
       <c r="H86">
         <v>19.899999999999999</v>
       </c>
-      <c r="I86" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J86" s="1">
         <v>44287</v>
       </c>
@@ -4624,9 +4408,6 @@
       <c r="H87">
         <v>5.9</v>
       </c>
-      <c r="I87" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J87" s="1">
         <v>44007</v>
       </c>
@@ -4674,9 +4455,6 @@
       <c r="H88">
         <v>17.2</v>
       </c>
-      <c r="I88" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J88" s="1">
         <v>44378</v>
       </c>
@@ -4724,9 +4502,6 @@
       <c r="H89">
         <v>10.4</v>
       </c>
-      <c r="I89" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J89" s="1">
         <v>44145</v>
       </c>
@@ -4771,9 +4546,6 @@
       <c r="H90">
         <v>25</v>
       </c>
-      <c r="I90" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J90" s="1">
         <v>44400</v>
       </c>
@@ -4821,9 +4593,6 @@
       <c r="H91">
         <v>21.7</v>
       </c>
-      <c r="I91" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J91" s="1">
         <v>44342</v>
       </c>
@@ -4871,9 +4640,6 @@
       <c r="H92">
         <v>12.3</v>
       </c>
-      <c r="I92" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J92" s="1">
         <v>43889</v>
       </c>
@@ -4921,9 +4687,6 @@
       <c r="H93">
         <v>8.6999999999999993</v>
       </c>
-      <c r="I93" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J93" s="1">
         <v>44470</v>
       </c>
@@ -4971,9 +4734,6 @@
       <c r="H94">
         <v>26.8</v>
       </c>
-      <c r="I94" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J94" s="1">
         <v>44173</v>
       </c>
@@ -5021,9 +4781,6 @@
       <c r="H95">
         <v>24.6</v>
       </c>
-      <c r="I95" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J95" s="1">
         <v>44069</v>
       </c>
@@ -5071,9 +4828,6 @@
       <c r="H96">
         <v>29.9</v>
       </c>
-      <c r="I96" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J96" s="1">
         <v>44243</v>
       </c>
@@ -5118,9 +4872,6 @@
       <c r="H97">
         <v>15.9</v>
       </c>
-      <c r="I97" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J97" s="1">
         <v>44139</v>
       </c>
@@ -5168,9 +4919,6 @@
       <c r="H98">
         <v>6.5</v>
       </c>
-      <c r="I98" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J98" s="1">
         <v>44281</v>
       </c>
@@ -5218,9 +4966,6 @@
       <c r="H99">
         <v>19.5</v>
       </c>
-      <c r="I99" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J99" s="1">
         <v>43909</v>
       </c>
@@ -5268,9 +5013,6 @@
       <c r="H100">
         <v>9.4</v>
       </c>
-      <c r="I100" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J100" s="1">
         <v>44005</v>
       </c>
@@ -5318,9 +5060,6 @@
       <c r="H101">
         <v>13.1</v>
       </c>
-      <c r="I101" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J101" s="1">
         <v>44273</v>
       </c>
@@ -5368,9 +5107,6 @@
       <c r="H102">
         <v>17.7</v>
       </c>
-      <c r="I102" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J102" s="1">
         <v>43867</v>
       </c>
@@ -5418,9 +5154,6 @@
       <c r="H103">
         <v>8.8000000000000007</v>
       </c>
-      <c r="I103" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J103" s="1">
         <v>44315</v>
       </c>
@@ -5468,9 +5201,6 @@
       <c r="H104">
         <v>15.2</v>
       </c>
-      <c r="I104" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J104" s="1">
         <v>44124</v>
       </c>
@@ -5518,9 +5248,6 @@
       <c r="H105">
         <v>9.5</v>
       </c>
-      <c r="I105" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J105" s="1">
         <v>44007</v>
       </c>
@@ -5568,9 +5295,6 @@
       <c r="H106">
         <v>8.4</v>
       </c>
-      <c r="I106" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J106" s="1">
         <v>44260</v>
       </c>
@@ -5618,9 +5342,6 @@
       <c r="H107">
         <v>9.6</v>
       </c>
-      <c r="I107" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J107" s="1">
         <v>44427</v>
       </c>
@@ -5668,9 +5389,6 @@
       <c r="H108">
         <v>25.3</v>
       </c>
-      <c r="I108" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J108" s="1">
         <v>43991</v>
       </c>
@@ -5718,9 +5436,6 @@
       <c r="H109">
         <v>12.6</v>
       </c>
-      <c r="I109" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J109" s="1">
         <v>44418</v>
       </c>
@@ -5768,9 +5483,6 @@
       <c r="H110">
         <v>21.7</v>
       </c>
-      <c r="I110" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J110" s="1">
         <v>44307</v>
       </c>
@@ -5818,9 +5530,6 @@
       <c r="H111">
         <v>25.1</v>
       </c>
-      <c r="I111" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J111" s="1">
         <v>44421</v>
       </c>
@@ -5868,9 +5577,6 @@
       <c r="H112">
         <v>16.399999999999999</v>
       </c>
-      <c r="I112" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J112" s="1">
         <v>44327</v>
       </c>
@@ -5918,9 +5624,6 @@
       <c r="H113">
         <v>9.6</v>
       </c>
-      <c r="I113" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J113" s="1">
         <v>44019</v>
       </c>
@@ -5968,9 +5671,6 @@
       <c r="H114">
         <v>13.2</v>
       </c>
-      <c r="I114" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J114" s="1">
         <v>44092</v>
       </c>
@@ -6018,9 +5718,6 @@
       <c r="H115">
         <v>19.3</v>
       </c>
-      <c r="I115" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="J115" s="1">
         <v>44040</v>
       </c>
@@ -6067,9 +5764,6 @@
       </c>
       <c r="H116">
         <v>14.3</v>
-      </c>
-      <c r="I116" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="J116" s="1">
         <v>44189</v>

</xml_diff>

<commit_message>
Fixed the "NA" values in YPwide2.xlsx and tweaks to YP-CORE_2_scores
</commit_message>
<xml_diff>
--- a/docs/YP-CORE/YPwide2.xlsx
+++ b/docs/YP-CORE/YPwide2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Current_share\Current_Data\MyR\shiny.psyctc.org\docs\YP-CORE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DE1A440-8D7A-40F6-B6E1-AF153E0E5532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6458EE3-5BA9-4EC5-9F62-33CB090D018E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14535" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="27">
   <si>
     <t>RespondentID</t>
   </si>
@@ -78,9 +78,6 @@
     <t>F</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>Ilustrates how app will create missing scoring if it has one scoring</t>
   </si>
   <si>
@@ -115,9 +112,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
-  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -147,10 +141,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -281,7 +275,7 @@
   <dimension ref="A1:P116"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -290,11 +284,11 @@
     <col min="2" max="2" width="10.85546875" customWidth="1"/>
     <col min="3" max="3" width="7.42578125" customWidth="1"/>
     <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="6" width="9.42578125" customWidth="1"/>
-    <col min="7" max="8" width="7.85546875" customWidth="1"/>
-    <col min="9" max="9" width="63" style="2" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" customWidth="1"/>
+    <col min="5" max="6" width="9.42578125" style="2" customWidth="1"/>
+    <col min="7" max="8" width="7.85546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="63" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" style="2" customWidth="1"/>
     <col min="12" max="12" width="17.28515625" customWidth="1"/>
     <col min="13" max="13" width="15.7109375" customWidth="1"/>
     <col min="14" max="14" width="18" customWidth="1"/>
@@ -327,7 +321,7 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J1" t="s">
@@ -365,26 +359,20 @@
       <c r="D2">
         <v>11</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>1.62</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="2">
         <v>1.1299999999999999</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="2">
         <v>16.2</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" s="1">
+      <c r="J2" s="2">
         <v>43924</v>
-      </c>
-      <c r="K2" t="s">
-        <v>17</v>
       </c>
       <c r="L2">
         <v>3</v>
@@ -415,26 +403,20 @@
       <c r="D3">
         <v>11</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <v>2.2599999999999998</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="2">
         <v>1.76</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" s="2">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H3">
-        <v>17.600000000000001</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" s="1">
+      <c r="J3" s="2">
         <v>43931</v>
-      </c>
-      <c r="K3" t="s">
-        <v>17</v>
       </c>
       <c r="L3">
         <v>7</v>
@@ -465,27 +447,24 @@
       <c r="D4">
         <v>12</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <v>1.9</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="2">
         <v>1.47</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="2">
         <v>19</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="2">
         <v>14.7</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" s="1">
+      <c r="I4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="2">
         <v>43915</v>
       </c>
-      <c r="K4" t="s">
-        <v>17</v>
-      </c>
       <c r="L4">
         <v>4</v>
       </c>
@@ -494,9 +473,6 @@
       </c>
       <c r="N4">
         <v>1</v>
-      </c>
-      <c r="O4" t="s">
-        <v>17</v>
       </c>
       <c r="P4">
         <v>5</v>
@@ -515,26 +491,20 @@
       <c r="D5">
         <v>13</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" s="2">
+        <v>1.32</v>
+      </c>
+      <c r="G5" s="2">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="H5" s="2">
+        <v>13.2</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F5">
-        <v>1.32</v>
-      </c>
-      <c r="G5">
-        <v>17.399999999999999</v>
-      </c>
-      <c r="H5">
-        <v>13.2</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" s="1">
+      <c r="J5" s="2">
         <v>44097</v>
-      </c>
-      <c r="K5" t="s">
-        <v>17</v>
       </c>
       <c r="L5">
         <v>8</v>
@@ -544,9 +514,6 @@
       </c>
       <c r="N5">
         <v>0</v>
-      </c>
-      <c r="O5" t="s">
-        <v>17</v>
       </c>
       <c r="P5">
         <v>10</v>
@@ -565,26 +532,11 @@
       <c r="D6">
         <v>14</v>
       </c>
-      <c r="E6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J6" s="1">
+      <c r="I6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="2">
         <v>44411</v>
-      </c>
-      <c r="K6" t="s">
-        <v>17</v>
       </c>
       <c r="L6">
         <v>1</v>
@@ -615,26 +567,17 @@
       <c r="D7">
         <v>15</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="2">
         <v>5</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="2">
         <v>2.0099999999999998</v>
       </c>
-      <c r="G7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J7" s="1">
+      <c r="I7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" s="2">
         <v>44174</v>
-      </c>
-      <c r="K7" t="s">
-        <v>17</v>
       </c>
       <c r="L7">
         <v>6</v>
@@ -665,26 +608,17 @@
       <c r="D8">
         <v>16</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="2">
         <v>-1</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="2">
         <v>2.92</v>
       </c>
-      <c r="G8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J8" s="1">
+      <c r="I8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" s="2">
         <v>44421</v>
-      </c>
-      <c r="K8" t="s">
-        <v>17</v>
       </c>
       <c r="L8">
         <v>3</v>
@@ -715,26 +649,17 @@
       <c r="D9">
         <v>17</v>
       </c>
-      <c r="E9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9">
+      <c r="G9" s="2">
         <v>56</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="2">
         <v>22.6</v>
       </c>
-      <c r="I9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J9" s="1">
+      <c r="I9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J9" s="2">
         <v>44036</v>
-      </c>
-      <c r="K9" t="s">
-        <v>17</v>
       </c>
       <c r="L9">
         <v>5</v>
@@ -765,26 +690,17 @@
       <c r="D10">
         <v>18</v>
       </c>
-      <c r="E10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10">
+      <c r="G10" s="2">
         <v>-1</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="2">
         <v>14.3</v>
       </c>
-      <c r="I10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J10" s="1">
+      <c r="I10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J10" s="2">
         <v>44167</v>
-      </c>
-      <c r="K10" t="s">
-        <v>17</v>
       </c>
       <c r="L10">
         <v>6</v>
@@ -810,31 +726,28 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11">
         <v>11</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="2">
         <v>1.62</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="2">
         <v>1.2</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="2">
         <v>16.2</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="2">
         <v>12</v>
       </c>
-      <c r="I11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J11" s="1">
+      <c r="I11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11" s="2">
         <v>44033</v>
-      </c>
-      <c r="K11" t="s">
-        <v>17</v>
       </c>
       <c r="L11">
         <v>6</v>
@@ -844,9 +757,6 @@
       </c>
       <c r="N11">
         <v>0</v>
-      </c>
-      <c r="O11" t="s">
-        <v>17</v>
       </c>
       <c r="P11">
         <v>6</v>
@@ -859,32 +769,26 @@
       <c r="B12">
         <v>1</v>
       </c>
-      <c r="C12" t="s">
-        <v>17</v>
-      </c>
       <c r="D12">
         <v>11</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="2">
         <v>1.62</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="2">
         <v>1.2</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="2">
         <v>16.2</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="2">
         <v>12</v>
       </c>
-      <c r="I12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J12" s="1">
+      <c r="I12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J12" s="2">
         <v>44147</v>
-      </c>
-      <c r="K12" t="s">
-        <v>17</v>
       </c>
       <c r="L12">
         <v>6</v>
@@ -910,31 +814,28 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D13">
         <v>11</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="2">
         <v>1.62</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="2">
         <v>1.2</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="2">
         <v>16.2</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="2">
         <v>12</v>
       </c>
-      <c r="I13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J13" s="1">
+      <c r="I13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J13" s="2">
         <v>43868</v>
-      </c>
-      <c r="K13" t="s">
-        <v>17</v>
       </c>
       <c r="L13">
         <v>5</v>
@@ -944,9 +845,6 @@
       </c>
       <c r="N13">
         <v>0</v>
-      </c>
-      <c r="O13" t="s">
-        <v>17</v>
       </c>
       <c r="P13">
         <v>7</v>
@@ -956,36 +854,27 @@
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
-        <v>17</v>
-      </c>
       <c r="C14" t="s">
         <v>16</v>
       </c>
-      <c r="D14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14">
+      <c r="E14" s="2">
         <v>3.87</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="2">
         <v>3.15</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="2">
         <v>38.700000000000003</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="2">
         <v>31.5</v>
       </c>
-      <c r="I14" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J14" s="1">
+      <c r="I14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J14" s="2">
         <v>44393</v>
       </c>
-      <c r="K14" t="s">
-        <v>17</v>
-      </c>
       <c r="L14">
         <v>1</v>
       </c>
@@ -994,9 +883,6 @@
       </c>
       <c r="N14">
         <v>1</v>
-      </c>
-      <c r="O14" t="s">
-        <v>17</v>
       </c>
       <c r="P14">
         <v>2</v>
@@ -1006,33 +892,27 @@
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
-        <v>17</v>
-      </c>
       <c r="C15" t="s">
         <v>16</v>
       </c>
       <c r="D15">
         <v>10</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="2">
         <v>3.87</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="2">
         <v>3.15</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="2">
         <v>38.700000000000003</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="2">
         <v>31.5</v>
       </c>
-      <c r="J15" s="1">
+      <c r="J15" s="2">
         <v>44434</v>
       </c>
-      <c r="K15" t="s">
-        <v>17</v>
-      </c>
       <c r="L15">
         <v>3</v>
       </c>
@@ -1041,9 +921,6 @@
       </c>
       <c r="N15">
         <v>0</v>
-      </c>
-      <c r="O15" t="s">
-        <v>17</v>
       </c>
       <c r="P15">
         <v>3</v>
@@ -1053,32 +930,26 @@
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
-        <v>17</v>
-      </c>
       <c r="C16" t="s">
         <v>16</v>
       </c>
       <c r="D16">
         <v>12</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="2">
         <v>3.87</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="2">
         <v>3.15</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="2">
         <v>38.700000000000003</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="2">
         <v>31.5</v>
       </c>
-      <c r="J16" s="1">
+      <c r="J16" s="2">
         <v>44204</v>
-      </c>
-      <c r="K16" t="s">
-        <v>17</v>
       </c>
       <c r="L16">
         <v>2</v>
@@ -1103,30 +974,9 @@
       <c r="B17">
         <v>1</v>
       </c>
-      <c r="C17" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E17" t="s">
-        <v>17</v>
-      </c>
-      <c r="F17" t="s">
-        <v>17</v>
-      </c>
-      <c r="G17" t="s">
-        <v>17</v>
-      </c>
-      <c r="H17" t="s">
-        <v>17</v>
-      </c>
-      <c r="J17" s="1">
+      <c r="J17" s="2">
         <v>43858</v>
       </c>
-      <c r="K17" t="s">
-        <v>17</v>
-      </c>
       <c r="L17">
         <v>3</v>
       </c>
@@ -1135,9 +985,6 @@
       </c>
       <c r="N17">
         <v>0</v>
-      </c>
-      <c r="O17" t="s">
-        <v>17</v>
       </c>
       <c r="P17">
         <v>4</v>
@@ -1151,28 +998,25 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D18">
         <v>11</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="2">
         <v>1.62</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="2">
         <v>1.2</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="2">
         <v>16.2</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="2">
         <v>12</v>
       </c>
-      <c r="J18" s="1">
+      <c r="J18" s="2">
         <v>44413</v>
-      </c>
-      <c r="K18" t="s">
-        <v>17</v>
       </c>
       <c r="L18">
         <v>3</v>
@@ -1203,24 +1047,21 @@
       <c r="D19">
         <v>12</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="2">
         <v>3.87</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="2">
         <v>3.15</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="2">
         <v>38.700000000000003</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="2">
         <v>31.5</v>
       </c>
-      <c r="J19" s="1">
+      <c r="J19" s="2">
         <v>44084</v>
       </c>
-      <c r="K19" t="s">
-        <v>17</v>
-      </c>
       <c r="L19">
         <v>3</v>
       </c>
@@ -1229,9 +1070,6 @@
       </c>
       <c r="N19">
         <v>0</v>
-      </c>
-      <c r="O19" t="s">
-        <v>17</v>
       </c>
       <c r="P19">
         <v>3</v>
@@ -1245,28 +1083,25 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D20">
         <v>12</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="2">
         <v>2.42</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="2">
         <v>1.79</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="2">
         <v>24.2</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="2">
         <v>17.899999999999999</v>
       </c>
-      <c r="J20" s="1">
+      <c r="J20" s="2">
         <v>44133</v>
-      </c>
-      <c r="K20" t="s">
-        <v>17</v>
       </c>
       <c r="L20">
         <v>10</v>
@@ -1297,23 +1132,20 @@
       <c r="D21">
         <v>13</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="2">
         <v>2.1800000000000002</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="2">
         <v>1.75</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="2">
         <v>21.8</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="2">
         <v>17.5</v>
       </c>
-      <c r="J21" s="1">
+      <c r="J21" s="2">
         <v>44470</v>
-      </c>
-      <c r="K21" t="s">
-        <v>17</v>
       </c>
       <c r="L21">
         <v>4</v>
@@ -1339,29 +1171,26 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D22">
         <v>13</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="2">
         <v>2.62</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="2">
         <v>2.09</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="2">
         <v>26.2</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="2">
         <v>20.9</v>
       </c>
-      <c r="J22" s="1">
+      <c r="J22" s="2">
         <v>44040</v>
       </c>
-      <c r="K22" t="s">
-        <v>17</v>
-      </c>
       <c r="L22">
         <v>4</v>
       </c>
@@ -1370,9 +1199,6 @@
       </c>
       <c r="N22">
         <v>1</v>
-      </c>
-      <c r="O22" t="s">
-        <v>17</v>
       </c>
       <c r="P22">
         <v>8</v>
@@ -1391,23 +1217,20 @@
       <c r="D23">
         <v>14</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="2">
         <v>1.27</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="2">
         <v>12.7</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="2">
         <v>11</v>
       </c>
-      <c r="J23" s="1">
+      <c r="J23" s="2">
         <v>44168</v>
-      </c>
-      <c r="K23" t="s">
-        <v>17</v>
       </c>
       <c r="L23">
         <v>9</v>
@@ -1433,28 +1256,25 @@
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D24">
         <v>14</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="2">
         <v>3.02</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="2">
         <v>2.38</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="2">
         <v>30.2</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="2">
         <v>23.8</v>
       </c>
-      <c r="J24" s="1">
+      <c r="J24" s="2">
         <v>44069</v>
-      </c>
-      <c r="K24" t="s">
-        <v>17</v>
       </c>
       <c r="L24">
         <v>8</v>
@@ -1464,9 +1284,6 @@
       </c>
       <c r="N24">
         <v>1</v>
-      </c>
-      <c r="O24" t="s">
-        <v>17</v>
       </c>
       <c r="P24">
         <v>9</v>
@@ -1485,23 +1302,20 @@
       <c r="D25">
         <v>15</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="2">
         <v>2.75</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="2">
         <v>2.23</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="2">
         <v>27.5</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="2">
         <v>22.3</v>
       </c>
-      <c r="J25" s="1">
+      <c r="J25" s="2">
         <v>44418</v>
-      </c>
-      <c r="K25" t="s">
-        <v>17</v>
       </c>
       <c r="L25">
         <v>5</v>
@@ -1511,9 +1325,6 @@
       </c>
       <c r="N25">
         <v>1</v>
-      </c>
-      <c r="O25" t="s">
-        <v>17</v>
       </c>
       <c r="P25">
         <v>8</v>
@@ -1527,29 +1338,26 @@
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D26">
         <v>15</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="2">
         <v>1.24</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="2">
         <v>1.08</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="2">
         <v>12.4</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="2">
         <v>10.8</v>
       </c>
-      <c r="J26" s="1">
+      <c r="J26" s="2">
         <v>44194</v>
       </c>
-      <c r="K26" t="s">
-        <v>17</v>
-      </c>
       <c r="L26">
         <v>4</v>
       </c>
@@ -1558,9 +1366,6 @@
       </c>
       <c r="N26">
         <v>1</v>
-      </c>
-      <c r="O26" t="s">
-        <v>17</v>
       </c>
       <c r="P26">
         <v>8</v>
@@ -1579,23 +1384,20 @@
       <c r="D27">
         <v>16</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="2">
         <v>1.4</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="2">
         <v>1.05</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="2">
         <v>14</v>
       </c>
-      <c r="H27">
+      <c r="H27" s="2">
         <v>10.5</v>
       </c>
-      <c r="J27" s="1">
+      <c r="J27" s="2">
         <v>44020</v>
-      </c>
-      <c r="K27" t="s">
-        <v>17</v>
       </c>
       <c r="L27">
         <v>5</v>
@@ -1605,9 +1407,6 @@
       </c>
       <c r="N27">
         <v>0</v>
-      </c>
-      <c r="O27" t="s">
-        <v>17</v>
       </c>
       <c r="P27">
         <v>5</v>
@@ -1621,28 +1420,25 @@
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D28">
         <v>16</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="2">
         <v>2.4700000000000002</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="2">
         <v>1.99</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="2">
         <v>24.7</v>
       </c>
-      <c r="H28">
+      <c r="H28" s="2">
         <v>19.899999999999999</v>
       </c>
-      <c r="J28" s="1">
+      <c r="J28" s="2">
         <v>43887</v>
-      </c>
-      <c r="K28" t="s">
-        <v>17</v>
       </c>
       <c r="L28">
         <v>6</v>
@@ -1673,24 +1469,21 @@
       <c r="D29">
         <v>17</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="2">
         <v>1.28</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="2">
         <v>0.92</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="2">
         <v>12.8</v>
       </c>
-      <c r="H29">
+      <c r="H29" s="2">
         <v>9.1999999999999993</v>
       </c>
-      <c r="J29" s="1">
+      <c r="J29" s="2">
         <v>44159</v>
       </c>
-      <c r="K29" t="s">
-        <v>17</v>
-      </c>
       <c r="L29">
         <v>3</v>
       </c>
@@ -1699,9 +1492,6 @@
       </c>
       <c r="N29">
         <v>0</v>
-      </c>
-      <c r="O29" t="s">
-        <v>17</v>
       </c>
       <c r="P29">
         <v>3</v>
@@ -1715,28 +1505,25 @@
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D30">
         <v>17</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="2">
         <v>3.17</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="2">
         <v>2.74</v>
       </c>
-      <c r="G30">
+      <c r="G30" s="2">
         <v>31.7</v>
       </c>
-      <c r="H30">
+      <c r="H30" s="2">
         <v>27.4</v>
       </c>
-      <c r="J30" s="1">
+      <c r="J30" s="2">
         <v>44244</v>
-      </c>
-      <c r="K30" t="s">
-        <v>17</v>
       </c>
       <c r="L30">
         <v>2</v>
@@ -1767,23 +1554,20 @@
       <c r="D31">
         <v>18</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="2">
         <v>1.82</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="2">
         <v>1.44</v>
       </c>
-      <c r="G31">
+      <c r="G31" s="2">
         <v>18.2</v>
       </c>
-      <c r="H31">
+      <c r="H31" s="2">
         <v>14.4</v>
       </c>
-      <c r="J31" s="1">
+      <c r="J31" s="2">
         <v>44236</v>
-      </c>
-      <c r="K31" t="s">
-        <v>17</v>
       </c>
       <c r="L31">
         <v>4</v>
@@ -1809,28 +1593,25 @@
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D32">
         <v>18</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="2">
         <v>2.95</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="2">
         <v>2.38</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="2">
         <v>29.5</v>
       </c>
-      <c r="H32">
+      <c r="H32" s="2">
         <v>23.8</v>
       </c>
-      <c r="J32" s="1">
+      <c r="J32" s="2">
         <v>44047</v>
-      </c>
-      <c r="K32" t="s">
-        <v>17</v>
       </c>
       <c r="L32">
         <v>4</v>
@@ -1861,22 +1642,22 @@
       <c r="D33">
         <v>13</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="2">
         <v>1.53</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="2">
         <v>1.31</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="2">
         <v>15.3</v>
       </c>
-      <c r="H33">
+      <c r="H33" s="2">
         <v>13.1</v>
       </c>
-      <c r="J33" s="1">
+      <c r="J33" s="2">
         <v>44124</v>
       </c>
-      <c r="K33" s="1">
+      <c r="K33" s="2">
         <v>44173</v>
       </c>
       <c r="L33">
@@ -1887,9 +1668,6 @@
       </c>
       <c r="N33">
         <v>1</v>
-      </c>
-      <c r="O33" t="s">
-        <v>17</v>
       </c>
       <c r="P33">
         <v>7</v>
@@ -1908,22 +1686,22 @@
       <c r="D34">
         <v>15</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="2">
         <v>2.4</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="2">
         <v>1.73</v>
       </c>
-      <c r="G34">
+      <c r="G34" s="2">
         <v>24</v>
       </c>
-      <c r="H34">
+      <c r="H34" s="2">
         <v>17.3</v>
       </c>
-      <c r="J34" s="1">
+      <c r="J34" s="2">
         <v>43935</v>
       </c>
-      <c r="K34" s="1">
+      <c r="K34" s="2">
         <v>43991</v>
       </c>
       <c r="L34">
@@ -1934,9 +1712,6 @@
       </c>
       <c r="N34">
         <v>0</v>
-      </c>
-      <c r="O34" t="s">
-        <v>17</v>
       </c>
       <c r="P34">
         <v>8</v>
@@ -1955,22 +1730,22 @@
       <c r="D35">
         <v>18</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="2">
         <v>2.25</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="2">
         <v>1.73</v>
       </c>
-      <c r="G35">
+      <c r="G35" s="2">
         <v>22.5</v>
       </c>
-      <c r="H35">
+      <c r="H35" s="2">
         <v>17.3</v>
       </c>
-      <c r="J35" s="1">
+      <c r="J35" s="2">
         <v>44127</v>
       </c>
-      <c r="K35" s="1">
+      <c r="K35" s="2">
         <v>44211</v>
       </c>
       <c r="L35">
@@ -1997,27 +1772,27 @@
         <v>2</v>
       </c>
       <c r="C36" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D36">
         <v>16</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="2">
         <v>2.29</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="2">
         <v>2.04</v>
       </c>
-      <c r="G36">
+      <c r="G36" s="2">
         <v>22.9</v>
       </c>
-      <c r="H36">
+      <c r="H36" s="2">
         <v>20.399999999999999</v>
       </c>
-      <c r="J36" s="1">
+      <c r="J36" s="2">
         <v>43893</v>
       </c>
-      <c r="K36" s="1">
+      <c r="K36" s="2">
         <v>43914</v>
       </c>
       <c r="L36">
@@ -2044,27 +1819,27 @@
         <v>4</v>
       </c>
       <c r="C37" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D37">
         <v>15</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="2">
         <v>1.62</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="2">
         <v>1.44</v>
       </c>
-      <c r="G37">
+      <c r="G37" s="2">
         <v>16.2</v>
       </c>
-      <c r="H37">
+      <c r="H37" s="2">
         <v>14.4</v>
       </c>
-      <c r="J37" s="1">
+      <c r="J37" s="2">
         <v>44238</v>
       </c>
-      <c r="K37" s="1">
+      <c r="K37" s="2">
         <v>44322</v>
       </c>
       <c r="L37">
@@ -2075,9 +1850,6 @@
       </c>
       <c r="N37">
         <v>0</v>
-      </c>
-      <c r="O37" t="s">
-        <v>17</v>
       </c>
       <c r="P37">
         <v>12</v>
@@ -2096,22 +1868,22 @@
       <c r="D38">
         <v>17</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="2">
         <v>2.34</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="2">
         <v>1.85</v>
       </c>
-      <c r="G38">
+      <c r="G38" s="2">
         <v>23.4</v>
       </c>
-      <c r="H38">
+      <c r="H38" s="2">
         <v>18.5</v>
       </c>
-      <c r="J38" s="1">
+      <c r="J38" s="2">
         <v>44166</v>
       </c>
-      <c r="K38" s="1">
+      <c r="K38" s="2">
         <v>44215</v>
       </c>
       <c r="L38">
@@ -2122,9 +1894,6 @@
       </c>
       <c r="N38">
         <v>0</v>
-      </c>
-      <c r="O38" t="s">
-        <v>17</v>
       </c>
       <c r="P38">
         <v>7</v>
@@ -2143,22 +1912,22 @@
       <c r="D39">
         <v>14</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="2">
         <v>2.42</v>
       </c>
-      <c r="F39">
+      <c r="F39" s="2">
         <v>1.9</v>
       </c>
-      <c r="G39">
+      <c r="G39" s="2">
         <v>24.2</v>
       </c>
-      <c r="H39">
+      <c r="H39" s="2">
         <v>19</v>
       </c>
-      <c r="J39" s="1">
+      <c r="J39" s="2">
         <v>44125</v>
       </c>
-      <c r="K39" s="1">
+      <c r="K39" s="2">
         <v>44188</v>
       </c>
       <c r="L39">
@@ -2169,9 +1938,6 @@
       </c>
       <c r="N39">
         <v>1</v>
-      </c>
-      <c r="O39" t="s">
-        <v>17</v>
       </c>
       <c r="P39">
         <v>9</v>
@@ -2185,27 +1951,27 @@
         <v>5</v>
       </c>
       <c r="C40" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D40">
         <v>13</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="2">
         <v>2.81</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="2">
         <v>2.34</v>
       </c>
-      <c r="G40">
+      <c r="G40" s="2">
         <v>28.1</v>
       </c>
-      <c r="H40">
+      <c r="H40" s="2">
         <v>23.4</v>
       </c>
-      <c r="J40" s="1">
+      <c r="J40" s="2">
         <v>44440</v>
       </c>
-      <c r="K40" s="1">
+      <c r="K40" s="2">
         <v>44482</v>
       </c>
       <c r="L40">
@@ -2216,9 +1982,6 @@
       </c>
       <c r="N40">
         <v>1</v>
-      </c>
-      <c r="O40" t="s">
-        <v>17</v>
       </c>
       <c r="P40">
         <v>6</v>
@@ -2237,22 +2000,22 @@
       <c r="D41">
         <v>13</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="2">
         <v>2.06</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="2">
         <v>1.62</v>
       </c>
-      <c r="G41">
+      <c r="G41" s="2">
         <v>20.6</v>
       </c>
-      <c r="H41">
+      <c r="H41" s="2">
         <v>16.2</v>
       </c>
-      <c r="J41" s="1">
+      <c r="J41" s="2">
         <v>43852</v>
       </c>
-      <c r="K41" s="1">
+      <c r="K41" s="2">
         <v>43915</v>
       </c>
       <c r="L41">
@@ -2279,27 +2042,27 @@
         <v>5</v>
       </c>
       <c r="C42" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D42">
         <v>15</v>
       </c>
-      <c r="E42">
+      <c r="E42" s="2">
         <v>1.94</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="2">
         <v>1.53</v>
       </c>
-      <c r="G42">
+      <c r="G42" s="2">
         <v>19.399999999999999</v>
       </c>
-      <c r="H42">
+      <c r="H42" s="2">
         <v>15.3</v>
       </c>
-      <c r="J42" s="1">
+      <c r="J42" s="2">
         <v>44209</v>
       </c>
-      <c r="K42" s="1">
+      <c r="K42" s="2">
         <v>44244</v>
       </c>
       <c r="L42">
@@ -2326,27 +2089,27 @@
         <v>4</v>
       </c>
       <c r="C43" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D43">
         <v>16</v>
       </c>
-      <c r="E43">
+      <c r="E43" s="2">
         <v>2.71</v>
       </c>
-      <c r="F43">
+      <c r="F43" s="2">
         <v>2.35</v>
       </c>
-      <c r="G43">
+      <c r="G43" s="2">
         <v>27.1</v>
       </c>
-      <c r="H43">
+      <c r="H43" s="2">
         <v>23.5</v>
       </c>
-      <c r="J43" s="1">
+      <c r="J43" s="2">
         <v>44287</v>
       </c>
-      <c r="K43" s="1">
+      <c r="K43" s="2">
         <v>44350</v>
       </c>
       <c r="L43">
@@ -2378,22 +2141,22 @@
       <c r="D44">
         <v>15</v>
       </c>
-      <c r="E44">
+      <c r="E44" s="2">
         <v>2.11</v>
       </c>
-      <c r="F44">
+      <c r="F44" s="2">
         <v>1.81</v>
       </c>
-      <c r="G44">
+      <c r="G44" s="2">
         <v>21.1</v>
       </c>
-      <c r="H44">
+      <c r="H44" s="2">
         <v>18.100000000000001</v>
       </c>
-      <c r="J44" s="1">
+      <c r="J44" s="2">
         <v>44125</v>
       </c>
-      <c r="K44" s="1">
+      <c r="K44" s="2">
         <v>44174</v>
       </c>
       <c r="L44">
@@ -2425,22 +2188,22 @@
       <c r="D45">
         <v>14</v>
       </c>
-      <c r="E45">
+      <c r="E45" s="2">
         <v>2.4300000000000002</v>
       </c>
-      <c r="F45">
+      <c r="F45" s="2">
         <v>2.08</v>
       </c>
-      <c r="G45">
+      <c r="G45" s="2">
         <v>24.3</v>
       </c>
-      <c r="H45">
+      <c r="H45" s="2">
         <v>20.8</v>
       </c>
-      <c r="J45" s="1">
+      <c r="J45" s="2">
         <v>44442</v>
       </c>
-      <c r="K45" s="1">
+      <c r="K45" s="2">
         <v>44477</v>
       </c>
       <c r="L45">
@@ -2472,22 +2235,22 @@
       <c r="D46">
         <v>15</v>
       </c>
-      <c r="E46">
+      <c r="E46" s="2">
         <v>0.92</v>
       </c>
-      <c r="F46">
+      <c r="F46" s="2">
         <v>0.68</v>
       </c>
-      <c r="G46">
+      <c r="G46" s="2">
         <v>9.1999999999999993</v>
       </c>
-      <c r="H46">
+      <c r="H46" s="2">
         <v>6.8</v>
       </c>
-      <c r="J46" s="1">
+      <c r="J46" s="2">
         <v>44251</v>
       </c>
-      <c r="K46" s="1">
+      <c r="K46" s="2">
         <v>44286</v>
       </c>
       <c r="L46">
@@ -2498,9 +2261,6 @@
       </c>
       <c r="N46">
         <v>0</v>
-      </c>
-      <c r="O46" t="s">
-        <v>17</v>
       </c>
       <c r="P46">
         <v>5</v>
@@ -2519,22 +2279,22 @@
       <c r="D47">
         <v>16</v>
       </c>
-      <c r="E47">
+      <c r="E47" s="2">
         <v>1.39</v>
       </c>
-      <c r="F47">
+      <c r="F47" s="2">
         <v>1.01</v>
       </c>
-      <c r="G47">
+      <c r="G47" s="2">
         <v>13.9</v>
       </c>
-      <c r="H47">
+      <c r="H47" s="2">
         <v>10.1</v>
       </c>
-      <c r="J47" s="1">
+      <c r="J47" s="2">
         <v>44469</v>
       </c>
-      <c r="K47" s="1">
+      <c r="K47" s="2">
         <v>44546</v>
       </c>
       <c r="L47">
@@ -2563,22 +2323,22 @@
       <c r="D48">
         <v>15</v>
       </c>
-      <c r="E48">
+      <c r="E48" s="2">
         <v>2.87</v>
       </c>
-      <c r="F48">
+      <c r="F48" s="2">
         <v>2.44</v>
       </c>
-      <c r="G48">
+      <c r="G48" s="2">
         <v>28.7</v>
       </c>
-      <c r="H48">
+      <c r="H48" s="2">
         <v>24.4</v>
       </c>
-      <c r="J48" s="1">
+      <c r="J48" s="2">
         <v>43846</v>
       </c>
-      <c r="K48" s="1">
+      <c r="K48" s="2">
         <v>43860</v>
       </c>
       <c r="L48">
@@ -2610,22 +2370,22 @@
       <c r="D49">
         <v>14</v>
       </c>
-      <c r="E49">
+      <c r="E49" s="2">
         <v>2.0699999999999998</v>
       </c>
-      <c r="F49">
+      <c r="F49" s="2">
         <v>1.67</v>
       </c>
-      <c r="G49">
+      <c r="G49" s="2">
         <v>20.7</v>
       </c>
-      <c r="H49">
+      <c r="H49" s="2">
         <v>16.7</v>
       </c>
-      <c r="J49" s="1">
+      <c r="J49" s="2">
         <v>44182</v>
       </c>
-      <c r="K49" s="1">
+      <c r="K49" s="2">
         <v>44203</v>
       </c>
       <c r="L49">
@@ -2636,9 +2396,6 @@
       </c>
       <c r="N49">
         <v>0</v>
-      </c>
-      <c r="O49" t="s">
-        <v>17</v>
       </c>
       <c r="P49">
         <v>3</v>
@@ -2652,27 +2409,27 @@
         <v>3</v>
       </c>
       <c r="C50" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D50">
         <v>17</v>
       </c>
-      <c r="E50">
+      <c r="E50" s="2">
         <v>1.48</v>
       </c>
-      <c r="F50">
+      <c r="F50" s="2">
         <v>1.26</v>
       </c>
-      <c r="G50">
+      <c r="G50" s="2">
         <v>14.8</v>
       </c>
-      <c r="H50">
+      <c r="H50" s="2">
         <v>12.6</v>
       </c>
-      <c r="J50" s="1">
+      <c r="J50" s="2">
         <v>44232</v>
       </c>
-      <c r="K50" s="1">
+      <c r="K50" s="2">
         <v>44274</v>
       </c>
       <c r="L50">
@@ -2683,9 +2440,6 @@
       </c>
       <c r="N50">
         <v>0</v>
-      </c>
-      <c r="O50" t="s">
-        <v>17</v>
       </c>
       <c r="P50">
         <v>6</v>
@@ -2699,27 +2453,27 @@
         <v>4</v>
       </c>
       <c r="C51" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D51">
         <v>18</v>
       </c>
-      <c r="E51">
+      <c r="E51" s="2">
         <v>0.72</v>
       </c>
-      <c r="F51">
+      <c r="F51" s="2">
         <v>0.65</v>
       </c>
-      <c r="G51">
+      <c r="G51" s="2">
         <v>7.2</v>
       </c>
-      <c r="H51">
+      <c r="H51" s="2">
         <v>6.5</v>
       </c>
-      <c r="J51" s="1">
+      <c r="J51" s="2">
         <v>44113</v>
       </c>
-      <c r="K51" s="1">
+      <c r="K51" s="2">
         <v>44141</v>
       </c>
       <c r="L51">
@@ -2751,22 +2505,22 @@
       <c r="D52">
         <v>13</v>
       </c>
-      <c r="E52">
+      <c r="E52" s="2">
         <v>0.99</v>
       </c>
-      <c r="F52">
+      <c r="F52" s="2">
         <v>0.7</v>
       </c>
-      <c r="G52">
+      <c r="G52" s="2">
         <v>9.9</v>
       </c>
-      <c r="H52">
+      <c r="H52" s="2">
         <v>7</v>
       </c>
-      <c r="J52" s="1">
+      <c r="J52" s="2">
         <v>44461</v>
       </c>
-      <c r="K52" s="1">
+      <c r="K52" s="2">
         <v>44482</v>
       </c>
       <c r="L52">
@@ -2777,9 +2531,6 @@
       </c>
       <c r="N52">
         <v>1</v>
-      </c>
-      <c r="O52" t="s">
-        <v>17</v>
       </c>
       <c r="P52">
         <v>3</v>
@@ -2793,27 +2544,27 @@
         <v>3</v>
       </c>
       <c r="C53" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D53">
         <v>15</v>
       </c>
-      <c r="E53">
+      <c r="E53" s="2">
         <v>2.0099999999999998</v>
       </c>
-      <c r="F53">
+      <c r="F53" s="2">
         <v>1.51</v>
       </c>
-      <c r="G53">
+      <c r="G53" s="2">
         <v>20.100000000000001</v>
       </c>
-      <c r="H53">
+      <c r="H53" s="2">
         <v>15.1</v>
       </c>
-      <c r="J53" s="1">
+      <c r="J53" s="2">
         <v>44209</v>
       </c>
-      <c r="K53" s="1">
+      <c r="K53" s="2">
         <v>44321</v>
       </c>
       <c r="L53">
@@ -2845,22 +2596,22 @@
       <c r="D54">
         <v>11</v>
       </c>
-      <c r="E54">
+      <c r="E54" s="2">
         <v>3.09</v>
       </c>
-      <c r="F54">
+      <c r="F54" s="2">
         <v>2.68</v>
       </c>
-      <c r="G54">
+      <c r="G54" s="2">
         <v>30.9</v>
       </c>
-      <c r="H54">
+      <c r="H54" s="2">
         <v>26.8</v>
       </c>
-      <c r="J54" s="1">
+      <c r="J54" s="2">
         <v>44462</v>
       </c>
-      <c r="K54" s="1">
+      <c r="K54" s="2">
         <v>44483</v>
       </c>
       <c r="L54">
@@ -2871,9 +2622,6 @@
       </c>
       <c r="N54">
         <v>0</v>
-      </c>
-      <c r="O54" t="s">
-        <v>17</v>
       </c>
       <c r="P54">
         <v>3</v>
@@ -2892,22 +2640,22 @@
       <c r="D55">
         <v>17</v>
       </c>
-      <c r="E55">
+      <c r="E55" s="2">
         <v>1.99</v>
       </c>
-      <c r="F55">
+      <c r="F55" s="2">
         <v>1.59</v>
       </c>
-      <c r="G55">
+      <c r="G55" s="2">
         <v>19.899999999999999</v>
       </c>
-      <c r="H55">
+      <c r="H55" s="2">
         <v>15.9</v>
       </c>
-      <c r="J55" s="1">
+      <c r="J55" s="2">
         <v>44084</v>
       </c>
-      <c r="K55" s="1">
+      <c r="K55" s="2">
         <v>44133</v>
       </c>
       <c r="L55">
@@ -2934,27 +2682,27 @@
         <v>4</v>
       </c>
       <c r="C56" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D56">
         <v>16</v>
       </c>
-      <c r="E56">
+      <c r="E56" s="2">
         <v>1.54</v>
       </c>
-      <c r="F56">
+      <c r="F56" s="2">
         <v>1.35</v>
       </c>
-      <c r="G56">
+      <c r="G56" s="2">
         <v>15.4</v>
       </c>
-      <c r="H56">
+      <c r="H56" s="2">
         <v>13.5</v>
       </c>
-      <c r="J56" s="1">
+      <c r="J56" s="2">
         <v>44337</v>
       </c>
-      <c r="K56" s="1">
+      <c r="K56" s="2">
         <v>44421</v>
       </c>
       <c r="L56">
@@ -2981,27 +2729,27 @@
         <v>2</v>
       </c>
       <c r="C57" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D57">
         <v>17</v>
       </c>
-      <c r="E57">
+      <c r="E57" s="2">
         <v>2.11</v>
       </c>
-      <c r="F57">
+      <c r="F57" s="2">
         <v>1.53</v>
       </c>
-      <c r="G57">
+      <c r="G57" s="2">
         <v>21.1</v>
       </c>
-      <c r="H57">
+      <c r="H57" s="2">
         <v>15.3</v>
       </c>
-      <c r="J57" s="1">
+      <c r="J57" s="2">
         <v>44400</v>
       </c>
-      <c r="K57" s="1">
+      <c r="K57" s="2">
         <v>44442</v>
       </c>
       <c r="L57">
@@ -3012,9 +2760,6 @@
       </c>
       <c r="N57">
         <v>1</v>
-      </c>
-      <c r="O57" t="s">
-        <v>17</v>
       </c>
       <c r="P57">
         <v>6</v>
@@ -3028,27 +2773,27 @@
         <v>4</v>
       </c>
       <c r="C58" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D58">
         <v>14</v>
       </c>
-      <c r="E58">
+      <c r="E58" s="2">
         <v>2.27</v>
       </c>
-      <c r="F58">
+      <c r="F58" s="2">
         <v>1.69</v>
       </c>
-      <c r="G58">
+      <c r="G58" s="2">
         <v>22.7</v>
       </c>
-      <c r="H58">
+      <c r="H58" s="2">
         <v>16.899999999999999</v>
       </c>
-      <c r="J58" s="1">
+      <c r="J58" s="2">
         <v>44420</v>
       </c>
-      <c r="K58" s="1">
+      <c r="K58" s="2">
         <v>44441</v>
       </c>
       <c r="L58">
@@ -3080,22 +2825,22 @@
       <c r="D59">
         <v>15</v>
       </c>
-      <c r="E59">
+      <c r="E59" s="2">
         <v>1.31</v>
       </c>
-      <c r="F59">
+      <c r="F59" s="2">
         <v>1.22</v>
       </c>
-      <c r="G59">
+      <c r="G59" s="2">
         <v>13.1</v>
       </c>
-      <c r="H59">
+      <c r="H59" s="2">
         <v>12.2</v>
       </c>
-      <c r="J59" s="1">
+      <c r="J59" s="2">
         <v>44330</v>
       </c>
-      <c r="K59" s="1">
+      <c r="K59" s="2">
         <v>44379</v>
       </c>
       <c r="L59">
@@ -3106,9 +2851,6 @@
       </c>
       <c r="N59">
         <v>0</v>
-      </c>
-      <c r="O59" t="s">
-        <v>17</v>
       </c>
       <c r="P59">
         <v>7</v>
@@ -3122,27 +2864,27 @@
         <v>4</v>
       </c>
       <c r="C60" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D60">
         <v>12</v>
       </c>
-      <c r="E60">
+      <c r="E60" s="2">
         <v>0.98</v>
       </c>
-      <c r="F60">
+      <c r="F60" s="2">
         <v>0.67</v>
       </c>
-      <c r="G60">
+      <c r="G60" s="2">
         <v>9.8000000000000007</v>
       </c>
-      <c r="H60">
+      <c r="H60" s="2">
         <v>6.7</v>
       </c>
-      <c r="J60" s="1">
+      <c r="J60" s="2">
         <v>43952</v>
       </c>
-      <c r="K60" s="1">
+      <c r="K60" s="2">
         <v>44001</v>
       </c>
       <c r="L60">
@@ -3169,27 +2911,27 @@
         <v>5</v>
       </c>
       <c r="C61" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D61">
         <v>12</v>
       </c>
-      <c r="E61">
+      <c r="E61" s="2">
         <v>3.08</v>
       </c>
-      <c r="F61">
+      <c r="F61" s="2">
         <v>2.65</v>
       </c>
-      <c r="G61">
+      <c r="G61" s="2">
         <v>30.8</v>
       </c>
-      <c r="H61">
+      <c r="H61" s="2">
         <v>26.5</v>
       </c>
-      <c r="J61" s="1">
+      <c r="J61" s="2">
         <v>44092</v>
       </c>
-      <c r="K61" s="1">
+      <c r="K61" s="2">
         <v>44113</v>
       </c>
       <c r="L61">
@@ -3200,9 +2942,6 @@
       </c>
       <c r="N61">
         <v>0</v>
-      </c>
-      <c r="O61" t="s">
-        <v>17</v>
       </c>
       <c r="P61">
         <v>3</v>
@@ -3221,22 +2960,22 @@
       <c r="D62">
         <v>11</v>
       </c>
-      <c r="E62">
+      <c r="E62" s="2">
         <v>2.94</v>
       </c>
-      <c r="F62">
+      <c r="F62" s="2">
         <v>2.2999999999999998</v>
       </c>
-      <c r="G62">
+      <c r="G62" s="2">
         <v>29.4</v>
       </c>
-      <c r="H62">
+      <c r="H62" s="2">
         <v>23</v>
       </c>
-      <c r="J62" s="1">
+      <c r="J62" s="2">
         <v>43861</v>
       </c>
-      <c r="K62" s="1">
+      <c r="K62" s="2">
         <v>43875</v>
       </c>
       <c r="L62">
@@ -3268,22 +3007,22 @@
       <c r="D63">
         <v>14</v>
       </c>
-      <c r="E63">
+      <c r="E63" s="2">
         <v>2.2599999999999998</v>
       </c>
-      <c r="F63">
+      <c r="F63" s="2">
         <v>1.85</v>
       </c>
-      <c r="G63">
+      <c r="G63" s="2">
         <v>22.6</v>
       </c>
-      <c r="H63">
+      <c r="H63" s="2">
         <v>18.5</v>
       </c>
-      <c r="J63" s="1">
+      <c r="J63" s="2">
         <v>43972</v>
       </c>
-      <c r="K63" s="1">
+      <c r="K63" s="2">
         <v>44014</v>
       </c>
       <c r="L63">
@@ -3294,9 +3033,6 @@
       </c>
       <c r="N63">
         <v>0</v>
-      </c>
-      <c r="O63" t="s">
-        <v>17</v>
       </c>
       <c r="P63">
         <v>6</v>
@@ -3310,27 +3046,27 @@
         <v>3</v>
       </c>
       <c r="C64" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D64">
         <v>14</v>
       </c>
-      <c r="E64">
+      <c r="E64" s="2">
         <v>1.46</v>
       </c>
-      <c r="F64">
+      <c r="F64" s="2">
         <v>1.05</v>
       </c>
-      <c r="G64">
+      <c r="G64" s="2">
         <v>14.6</v>
       </c>
-      <c r="H64">
+      <c r="H64" s="2">
         <v>10.5</v>
       </c>
-      <c r="J64" s="1">
+      <c r="J64" s="2">
         <v>44370</v>
       </c>
-      <c r="K64" s="1">
+      <c r="K64" s="2">
         <v>44426</v>
       </c>
       <c r="L64">
@@ -3362,22 +3098,22 @@
       <c r="D65">
         <v>16</v>
       </c>
-      <c r="E65">
+      <c r="E65" s="2">
         <v>2.59</v>
       </c>
-      <c r="F65">
+      <c r="F65" s="2">
         <v>2.34</v>
       </c>
-      <c r="G65">
+      <c r="G65" s="2">
         <v>25.9</v>
       </c>
-      <c r="H65">
+      <c r="H65" s="2">
         <v>23.4</v>
       </c>
-      <c r="J65" s="1">
+      <c r="J65" s="2">
         <v>44252</v>
       </c>
-      <c r="K65" s="1">
+      <c r="K65" s="2">
         <v>44322</v>
       </c>
       <c r="L65">
@@ -3388,9 +3124,6 @@
       </c>
       <c r="N65">
         <v>0</v>
-      </c>
-      <c r="O65" t="s">
-        <v>17</v>
       </c>
       <c r="P65">
         <v>10</v>
@@ -3409,22 +3142,22 @@
       <c r="D66">
         <v>14</v>
       </c>
-      <c r="E66">
+      <c r="E66" s="2">
         <v>3.55</v>
       </c>
-      <c r="F66">
+      <c r="F66" s="2">
         <v>2.76</v>
       </c>
-      <c r="G66">
+      <c r="G66" s="2">
         <v>35.5</v>
       </c>
-      <c r="H66">
+      <c r="H66" s="2">
         <v>27.6</v>
       </c>
-      <c r="J66" s="1">
+      <c r="J66" s="2">
         <v>43875</v>
       </c>
-      <c r="K66" s="1">
+      <c r="K66" s="2">
         <v>43924</v>
       </c>
       <c r="L66">
@@ -3451,27 +3184,27 @@
         <v>4</v>
       </c>
       <c r="C67" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D67">
         <v>15</v>
       </c>
-      <c r="E67">
+      <c r="E67" s="2">
         <v>1.99</v>
       </c>
-      <c r="F67">
+      <c r="F67" s="2">
         <v>1.66</v>
       </c>
-      <c r="G67">
+      <c r="G67" s="2">
         <v>19.899999999999999</v>
       </c>
-      <c r="H67">
+      <c r="H67" s="2">
         <v>16.600000000000001</v>
       </c>
-      <c r="J67" s="1">
+      <c r="J67" s="2">
         <v>44083</v>
       </c>
-      <c r="K67" s="1">
+      <c r="K67" s="2">
         <v>44132</v>
       </c>
       <c r="L67">
@@ -3482,9 +3215,6 @@
       </c>
       <c r="N67">
         <v>0</v>
-      </c>
-      <c r="O67" t="s">
-        <v>17</v>
       </c>
       <c r="P67">
         <v>7</v>
@@ -3498,27 +3228,27 @@
         <v>5</v>
       </c>
       <c r="C68" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D68">
         <v>13</v>
       </c>
-      <c r="E68">
+      <c r="E68" s="2">
         <v>3.19</v>
       </c>
-      <c r="F68">
+      <c r="F68" s="2">
         <v>2.4300000000000002</v>
       </c>
-      <c r="G68">
+      <c r="G68" s="2">
         <v>31.9</v>
       </c>
-      <c r="H68">
+      <c r="H68" s="2">
         <v>24.3</v>
       </c>
-      <c r="J68" s="1">
+      <c r="J68" s="2">
         <v>43854</v>
       </c>
-      <c r="K68" s="1">
+      <c r="K68" s="2">
         <v>43896</v>
       </c>
       <c r="L68">
@@ -3529,9 +3259,6 @@
       </c>
       <c r="N68">
         <v>0</v>
-      </c>
-      <c r="O68" t="s">
-        <v>17</v>
       </c>
       <c r="P68">
         <v>6</v>
@@ -3550,22 +3277,22 @@
       <c r="D69">
         <v>13</v>
       </c>
-      <c r="E69">
+      <c r="E69" s="2">
         <v>0.78</v>
       </c>
-      <c r="F69">
+      <c r="F69" s="2">
         <v>0.56000000000000005</v>
       </c>
-      <c r="G69">
+      <c r="G69" s="2">
         <v>7.8</v>
       </c>
-      <c r="H69">
+      <c r="H69" s="2">
         <v>5.6</v>
       </c>
-      <c r="J69" s="1">
+      <c r="J69" s="2">
         <v>44166</v>
       </c>
-      <c r="K69" s="1">
+      <c r="K69" s="2">
         <v>44180</v>
       </c>
       <c r="L69">
@@ -3592,27 +3319,27 @@
         <v>3</v>
       </c>
       <c r="C70" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D70">
         <v>17</v>
       </c>
-      <c r="E70">
+      <c r="E70" s="2">
         <v>2.9</v>
       </c>
-      <c r="F70">
+      <c r="F70" s="2">
         <v>2.2799999999999998</v>
       </c>
-      <c r="G70">
+      <c r="G70" s="2">
         <v>29</v>
       </c>
-      <c r="H70">
+      <c r="H70" s="2">
         <v>22.8</v>
       </c>
-      <c r="J70" s="1">
+      <c r="J70" s="2">
         <v>44370</v>
       </c>
-      <c r="K70" s="1">
+      <c r="K70" s="2">
         <v>44398</v>
       </c>
       <c r="L70">
@@ -3623,9 +3350,6 @@
       </c>
       <c r="N70">
         <v>0</v>
-      </c>
-      <c r="O70" t="s">
-        <v>17</v>
       </c>
       <c r="P70">
         <v>4</v>
@@ -3639,27 +3363,27 @@
         <v>2</v>
       </c>
       <c r="C71" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D71">
         <v>14</v>
       </c>
-      <c r="E71">
+      <c r="E71" s="2">
         <v>2.72</v>
       </c>
-      <c r="F71">
+      <c r="F71" s="2">
         <v>2.17</v>
       </c>
-      <c r="G71">
+      <c r="G71" s="2">
         <v>27.2</v>
       </c>
-      <c r="H71">
+      <c r="H71" s="2">
         <v>21.7</v>
       </c>
-      <c r="J71" s="1">
+      <c r="J71" s="2">
         <v>44412</v>
       </c>
-      <c r="K71" s="1">
+      <c r="K71" s="2">
         <v>44545</v>
       </c>
       <c r="L71">
@@ -3670,9 +3394,6 @@
       </c>
       <c r="N71">
         <v>1</v>
-      </c>
-      <c r="O71" t="s">
-        <v>17</v>
       </c>
       <c r="P71">
         <v>19</v>
@@ -3691,22 +3412,22 @@
       <c r="D72">
         <v>18</v>
       </c>
-      <c r="E72">
+      <c r="E72" s="2">
         <v>1.08</v>
       </c>
-      <c r="F72">
+      <c r="F72" s="2">
         <v>0.81</v>
       </c>
-      <c r="G72">
+      <c r="G72" s="2">
         <v>10.8</v>
       </c>
-      <c r="H72">
+      <c r="H72" s="2">
         <v>8.1</v>
       </c>
-      <c r="J72" s="1">
+      <c r="J72" s="2">
         <v>44007</v>
       </c>
-      <c r="K72" s="1">
+      <c r="K72" s="2">
         <v>44021</v>
       </c>
       <c r="L72">
@@ -3733,27 +3454,27 @@
         <v>3</v>
       </c>
       <c r="C73" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D73">
         <v>15</v>
       </c>
-      <c r="E73">
+      <c r="E73" s="2">
         <v>1.95</v>
       </c>
-      <c r="F73">
+      <c r="F73" s="2">
         <v>1.41</v>
       </c>
-      <c r="G73">
+      <c r="G73" s="2">
         <v>19.5</v>
       </c>
-      <c r="H73">
+      <c r="H73" s="2">
         <v>14.1</v>
       </c>
-      <c r="J73" s="1">
+      <c r="J73" s="2">
         <v>44287</v>
       </c>
-      <c r="K73" s="1">
+      <c r="K73" s="2">
         <v>44315</v>
       </c>
       <c r="L73">
@@ -3764,9 +3485,6 @@
       </c>
       <c r="N73">
         <v>0</v>
-      </c>
-      <c r="O73" t="s">
-        <v>17</v>
       </c>
       <c r="P73">
         <v>4</v>
@@ -3785,22 +3503,22 @@
       <c r="D74">
         <v>16</v>
       </c>
-      <c r="E74">
+      <c r="E74" s="2">
         <v>2.25</v>
       </c>
-      <c r="F74">
+      <c r="F74" s="2">
         <v>1.91</v>
       </c>
-      <c r="G74">
+      <c r="G74" s="2">
         <v>22.5</v>
       </c>
-      <c r="H74">
+      <c r="H74" s="2">
         <v>19.100000000000001</v>
       </c>
-      <c r="J74" s="1">
+      <c r="J74" s="2">
         <v>44321</v>
       </c>
-      <c r="K74" s="1">
+      <c r="K74" s="2">
         <v>44342</v>
       </c>
       <c r="L74">
@@ -3811,9 +3529,6 @@
       </c>
       <c r="N74">
         <v>0</v>
-      </c>
-      <c r="O74" t="s">
-        <v>17</v>
       </c>
       <c r="P74">
         <v>3</v>
@@ -3832,22 +3547,22 @@
       <c r="D75">
         <v>15</v>
       </c>
-      <c r="E75">
+      <c r="E75" s="2">
         <v>1.01</v>
       </c>
-      <c r="F75">
+      <c r="F75" s="2">
         <v>0.91</v>
       </c>
-      <c r="G75">
+      <c r="G75" s="2">
         <v>10.1</v>
       </c>
-      <c r="H75">
+      <c r="H75" s="2">
         <v>9.1</v>
       </c>
-      <c r="J75" s="1">
+      <c r="J75" s="2">
         <v>44056</v>
       </c>
-      <c r="K75" s="1">
+      <c r="K75" s="2">
         <v>44161</v>
       </c>
       <c r="L75">
@@ -3858,9 +3573,6 @@
       </c>
       <c r="N75">
         <v>1</v>
-      </c>
-      <c r="O75" t="s">
-        <v>17</v>
       </c>
       <c r="P75">
         <v>15</v>
@@ -3874,27 +3586,27 @@
         <v>3</v>
       </c>
       <c r="C76" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D76">
         <v>16</v>
       </c>
-      <c r="E76">
+      <c r="E76" s="2">
         <v>2.67</v>
       </c>
-      <c r="F76">
+      <c r="F76" s="2">
         <v>2.15</v>
       </c>
-      <c r="G76">
+      <c r="G76" s="2">
         <v>26.7</v>
       </c>
-      <c r="H76">
+      <c r="H76" s="2">
         <v>21.5</v>
       </c>
-      <c r="J76" s="1">
+      <c r="J76" s="2">
         <v>44134</v>
       </c>
-      <c r="K76" s="1">
+      <c r="K76" s="2">
         <v>44176</v>
       </c>
       <c r="L76">
@@ -3905,9 +3617,6 @@
       </c>
       <c r="N76">
         <v>0</v>
-      </c>
-      <c r="O76" t="s">
-        <v>17</v>
       </c>
       <c r="P76">
         <v>6</v>
@@ -3926,22 +3635,22 @@
       <c r="D77">
         <v>15</v>
       </c>
-      <c r="E77">
+      <c r="E77" s="2">
         <v>2.91</v>
       </c>
-      <c r="F77">
+      <c r="F77" s="2">
         <v>2.2400000000000002</v>
       </c>
-      <c r="G77">
+      <c r="G77" s="2">
         <v>29.1</v>
       </c>
-      <c r="H77">
+      <c r="H77" s="2">
         <v>22.4</v>
       </c>
-      <c r="J77" s="1">
+      <c r="J77" s="2">
         <v>43949</v>
       </c>
-      <c r="K77" s="1">
+      <c r="K77" s="2">
         <v>43977</v>
       </c>
       <c r="L77">
@@ -3952,9 +3661,6 @@
       </c>
       <c r="N77">
         <v>0</v>
-      </c>
-      <c r="O77" t="s">
-        <v>17</v>
       </c>
       <c r="P77">
         <v>4</v>
@@ -3973,22 +3679,22 @@
       <c r="D78">
         <v>16</v>
       </c>
-      <c r="E78">
+      <c r="E78" s="2">
         <v>3.14</v>
       </c>
-      <c r="F78">
+      <c r="F78" s="2">
         <v>2.6</v>
       </c>
-      <c r="G78">
+      <c r="G78" s="2">
         <v>31.4</v>
       </c>
-      <c r="H78">
+      <c r="H78" s="2">
         <v>26</v>
       </c>
-      <c r="J78" s="1">
+      <c r="J78" s="2">
         <v>44180</v>
       </c>
-      <c r="K78" s="1">
+      <c r="K78" s="2">
         <v>44215</v>
       </c>
       <c r="L78">
@@ -3999,9 +3705,6 @@
       </c>
       <c r="N78">
         <v>1</v>
-      </c>
-      <c r="O78" t="s">
-        <v>17</v>
       </c>
       <c r="P78">
         <v>5</v>
@@ -4020,22 +3723,22 @@
       <c r="D79">
         <v>13</v>
       </c>
-      <c r="E79">
+      <c r="E79" s="2">
         <v>2.93</v>
       </c>
-      <c r="F79">
+      <c r="F79" s="2">
         <v>2.39</v>
       </c>
-      <c r="G79">
+      <c r="G79" s="2">
         <v>29.3</v>
       </c>
-      <c r="H79">
+      <c r="H79" s="2">
         <v>23.9</v>
       </c>
-      <c r="J79" s="1">
+      <c r="J79" s="2">
         <v>43984</v>
       </c>
-      <c r="K79" s="1">
+      <c r="K79" s="2">
         <v>44089</v>
       </c>
       <c r="L79">
@@ -4046,9 +3749,6 @@
       </c>
       <c r="N79">
         <v>1</v>
-      </c>
-      <c r="O79" t="s">
-        <v>17</v>
       </c>
       <c r="P79">
         <v>15</v>
@@ -4062,27 +3762,27 @@
         <v>2</v>
       </c>
       <c r="C80" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D80">
         <v>15</v>
       </c>
-      <c r="E80">
+      <c r="E80" s="2">
         <v>3.79</v>
       </c>
-      <c r="F80">
+      <c r="F80" s="2">
         <v>3.01</v>
       </c>
-      <c r="G80">
+      <c r="G80" s="2">
         <v>37.9</v>
       </c>
-      <c r="H80">
+      <c r="H80" s="2">
         <v>30.1</v>
       </c>
-      <c r="J80" s="1">
+      <c r="J80" s="2">
         <v>43943</v>
       </c>
-      <c r="K80" s="1">
+      <c r="K80" s="2">
         <v>43999</v>
       </c>
       <c r="L80">
@@ -4093,9 +3793,6 @@
       </c>
       <c r="N80">
         <v>0</v>
-      </c>
-      <c r="O80" t="s">
-        <v>17</v>
       </c>
       <c r="P80">
         <v>8</v>
@@ -4109,27 +3806,27 @@
         <v>5</v>
       </c>
       <c r="C81" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D81">
         <v>17</v>
       </c>
-      <c r="E81">
+      <c r="E81" s="2">
         <v>2.42</v>
       </c>
-      <c r="F81">
+      <c r="F81" s="2">
         <v>1.87</v>
       </c>
-      <c r="G81">
+      <c r="G81" s="2">
         <v>24.2</v>
       </c>
-      <c r="H81">
+      <c r="H81" s="2">
         <v>18.7</v>
       </c>
-      <c r="J81" s="1">
+      <c r="J81" s="2">
         <v>44084</v>
       </c>
-      <c r="K81" s="1">
+      <c r="K81" s="2">
         <v>44119</v>
       </c>
       <c r="L81">
@@ -4140,9 +3837,6 @@
       </c>
       <c r="N81">
         <v>0</v>
-      </c>
-      <c r="O81" t="s">
-        <v>17</v>
       </c>
       <c r="P81">
         <v>5</v>
@@ -4156,27 +3850,27 @@
         <v>2</v>
       </c>
       <c r="C82" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D82">
         <v>13</v>
       </c>
-      <c r="E82">
+      <c r="E82" s="2">
         <v>2.65</v>
       </c>
-      <c r="F82">
+      <c r="F82" s="2">
         <v>2.23</v>
       </c>
-      <c r="G82">
+      <c r="G82" s="2">
         <v>26.5</v>
       </c>
-      <c r="H82">
+      <c r="H82" s="2">
         <v>22.3</v>
       </c>
-      <c r="J82" s="1">
+      <c r="J82" s="2">
         <v>44028</v>
       </c>
-      <c r="K82" s="1">
+      <c r="K82" s="2">
         <v>44077</v>
       </c>
       <c r="L82">
@@ -4187,9 +3881,6 @@
       </c>
       <c r="N82">
         <v>0</v>
-      </c>
-      <c r="O82" t="s">
-        <v>17</v>
       </c>
       <c r="P82">
         <v>7</v>
@@ -4208,22 +3899,22 @@
       <c r="D83">
         <v>16</v>
       </c>
-      <c r="E83">
+      <c r="E83" s="2">
         <v>1.98</v>
       </c>
-      <c r="F83">
+      <c r="F83" s="2">
         <v>1.77</v>
       </c>
-      <c r="G83">
+      <c r="G83" s="2">
         <v>19.8</v>
       </c>
-      <c r="H83">
+      <c r="H83" s="2">
         <v>17.7</v>
       </c>
-      <c r="J83" s="1">
+      <c r="J83" s="2">
         <v>44463</v>
       </c>
-      <c r="K83" s="1">
+      <c r="K83" s="2">
         <v>44505</v>
       </c>
       <c r="L83">
@@ -4234,9 +3925,6 @@
       </c>
       <c r="N83">
         <v>0</v>
-      </c>
-      <c r="O83" t="s">
-        <v>17</v>
       </c>
       <c r="P83">
         <v>6</v>
@@ -4250,27 +3938,27 @@
         <v>3</v>
       </c>
       <c r="C84" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D84">
         <v>17</v>
       </c>
-      <c r="E84">
+      <c r="E84" s="2">
         <v>3.11</v>
       </c>
-      <c r="F84">
+      <c r="F84" s="2">
         <v>2.4</v>
       </c>
-      <c r="G84">
+      <c r="G84" s="2">
         <v>31.1</v>
       </c>
-      <c r="H84">
+      <c r="H84" s="2">
         <v>24</v>
       </c>
-      <c r="J84" s="1">
+      <c r="J84" s="2">
         <v>44435</v>
       </c>
-      <c r="K84" s="1">
+      <c r="K84" s="2">
         <v>44463</v>
       </c>
       <c r="L84">
@@ -4302,22 +3990,22 @@
       <c r="D85">
         <v>16</v>
       </c>
-      <c r="E85">
+      <c r="E85" s="2">
         <v>3.05</v>
       </c>
-      <c r="F85">
+      <c r="F85" s="2">
         <v>2.2999999999999998</v>
       </c>
-      <c r="G85">
+      <c r="G85" s="2">
         <v>30.5</v>
       </c>
-      <c r="H85">
+      <c r="H85" s="2">
         <v>23</v>
       </c>
-      <c r="J85" s="1">
+      <c r="J85" s="2">
         <v>44252</v>
       </c>
-      <c r="K85" s="1">
+      <c r="K85" s="2">
         <v>44301</v>
       </c>
       <c r="L85">
@@ -4328,9 +4016,6 @@
       </c>
       <c r="N85">
         <v>0</v>
-      </c>
-      <c r="O85" t="s">
-        <v>17</v>
       </c>
       <c r="P85">
         <v>7</v>
@@ -4349,22 +4034,22 @@
       <c r="D86">
         <v>17</v>
       </c>
-      <c r="E86">
+      <c r="E86" s="2">
         <v>2.36</v>
       </c>
-      <c r="F86">
+      <c r="F86" s="2">
         <v>1.99</v>
       </c>
-      <c r="G86">
+      <c r="G86" s="2">
         <v>23.6</v>
       </c>
-      <c r="H86">
+      <c r="H86" s="2">
         <v>19.899999999999999</v>
       </c>
-      <c r="J86" s="1">
+      <c r="J86" s="2">
         <v>44287</v>
       </c>
-      <c r="K86" s="1">
+      <c r="K86" s="2">
         <v>44329</v>
       </c>
       <c r="L86">
@@ -4396,22 +4081,22 @@
       <c r="D87">
         <v>15</v>
       </c>
-      <c r="E87">
+      <c r="E87" s="2">
         <v>1.08</v>
       </c>
-      <c r="F87">
+      <c r="F87" s="2">
         <v>0.59</v>
       </c>
-      <c r="G87">
+      <c r="G87" s="2">
         <v>10.8</v>
       </c>
-      <c r="H87">
+      <c r="H87" s="2">
         <v>5.9</v>
       </c>
-      <c r="J87" s="1">
+      <c r="J87" s="2">
         <v>44007</v>
       </c>
-      <c r="K87" s="1">
+      <c r="K87" s="2">
         <v>44056</v>
       </c>
       <c r="L87">
@@ -4438,27 +4123,27 @@
         <v>3</v>
       </c>
       <c r="C88" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D88">
         <v>18</v>
       </c>
-      <c r="E88">
+      <c r="E88" s="2">
         <v>2.23</v>
       </c>
-      <c r="F88">
+      <c r="F88" s="2">
         <v>1.72</v>
       </c>
-      <c r="G88">
+      <c r="G88" s="2">
         <v>22.3</v>
       </c>
-      <c r="H88">
+      <c r="H88" s="2">
         <v>17.2</v>
       </c>
-      <c r="J88" s="1">
+      <c r="J88" s="2">
         <v>44378</v>
       </c>
-      <c r="K88" s="1">
+      <c r="K88" s="2">
         <v>44399</v>
       </c>
       <c r="L88">
@@ -4485,27 +4170,27 @@
         <v>5</v>
       </c>
       <c r="C89" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D89">
         <v>11</v>
       </c>
-      <c r="E89">
+      <c r="E89" s="2">
         <v>1.25</v>
       </c>
-      <c r="F89">
+      <c r="F89" s="2">
         <v>1.04</v>
       </c>
-      <c r="G89">
+      <c r="G89" s="2">
         <v>12.5</v>
       </c>
-      <c r="H89">
+      <c r="H89" s="2">
         <v>10.4</v>
       </c>
-      <c r="J89" s="1">
+      <c r="J89" s="2">
         <v>44145</v>
       </c>
-      <c r="K89" s="1">
+      <c r="K89" s="2">
         <v>44180</v>
       </c>
       <c r="L89">
@@ -4534,22 +4219,22 @@
       <c r="D90">
         <v>14</v>
       </c>
-      <c r="E90">
+      <c r="E90" s="2">
         <v>2.88</v>
       </c>
-      <c r="F90">
+      <c r="F90" s="2">
         <v>2.5</v>
       </c>
-      <c r="G90">
+      <c r="G90" s="2">
         <v>28.8</v>
       </c>
-      <c r="H90">
+      <c r="H90" s="2">
         <v>25</v>
       </c>
-      <c r="J90" s="1">
+      <c r="J90" s="2">
         <v>44400</v>
       </c>
-      <c r="K90" s="1">
+      <c r="K90" s="2">
         <v>44442</v>
       </c>
       <c r="L90">
@@ -4576,27 +4261,27 @@
         <v>4</v>
       </c>
       <c r="C91" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D91">
         <v>13</v>
       </c>
-      <c r="E91">
+      <c r="E91" s="2">
         <v>2.96</v>
       </c>
-      <c r="F91">
+      <c r="F91" s="2">
         <v>2.17</v>
       </c>
-      <c r="G91">
+      <c r="G91" s="2">
         <v>29.6</v>
       </c>
-      <c r="H91">
+      <c r="H91" s="2">
         <v>21.7</v>
       </c>
-      <c r="J91" s="1">
+      <c r="J91" s="2">
         <v>44342</v>
       </c>
-      <c r="K91" s="1">
+      <c r="K91" s="2">
         <v>44370</v>
       </c>
       <c r="L91">
@@ -4623,27 +4308,27 @@
         <v>3</v>
       </c>
       <c r="C92" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D92">
         <v>15</v>
       </c>
-      <c r="E92">
+      <c r="E92" s="2">
         <v>1.54</v>
       </c>
-      <c r="F92">
+      <c r="F92" s="2">
         <v>1.23</v>
       </c>
-      <c r="G92">
+      <c r="G92" s="2">
         <v>15.4</v>
       </c>
-      <c r="H92">
+      <c r="H92" s="2">
         <v>12.3</v>
       </c>
-      <c r="J92" s="1">
+      <c r="J92" s="2">
         <v>43889</v>
       </c>
-      <c r="K92" s="1">
+      <c r="K92" s="2">
         <v>43945</v>
       </c>
       <c r="L92">
@@ -4654,9 +4339,6 @@
       </c>
       <c r="N92">
         <v>2</v>
-      </c>
-      <c r="O92" t="s">
-        <v>17</v>
       </c>
       <c r="P92">
         <v>8</v>
@@ -4675,22 +4357,22 @@
       <c r="D93">
         <v>16</v>
       </c>
-      <c r="E93">
+      <c r="E93" s="2">
         <v>1.32</v>
       </c>
-      <c r="F93">
+      <c r="F93" s="2">
         <v>0.87</v>
       </c>
-      <c r="G93">
+      <c r="G93" s="2">
         <v>13.2</v>
       </c>
-      <c r="H93">
+      <c r="H93" s="2">
         <v>8.6999999999999993</v>
       </c>
-      <c r="J93" s="1">
+      <c r="J93" s="2">
         <v>44470</v>
       </c>
-      <c r="K93" s="1">
+      <c r="K93" s="2">
         <v>44505</v>
       </c>
       <c r="L93">
@@ -4701,9 +4383,6 @@
       </c>
       <c r="N93">
         <v>0</v>
-      </c>
-      <c r="O93" t="s">
-        <v>17</v>
       </c>
       <c r="P93">
         <v>5</v>
@@ -4717,27 +4396,27 @@
         <v>3</v>
       </c>
       <c r="C94" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D94">
         <v>13</v>
       </c>
-      <c r="E94">
+      <c r="E94" s="2">
         <v>3.13</v>
       </c>
-      <c r="F94">
+      <c r="F94" s="2">
         <v>2.68</v>
       </c>
-      <c r="G94">
+      <c r="G94" s="2">
         <v>31.3</v>
       </c>
-      <c r="H94">
+      <c r="H94" s="2">
         <v>26.8</v>
       </c>
-      <c r="J94" s="1">
+      <c r="J94" s="2">
         <v>44173</v>
       </c>
-      <c r="K94" s="1">
+      <c r="K94" s="2">
         <v>44222</v>
       </c>
       <c r="L94">
@@ -4764,27 +4443,27 @@
         <v>2</v>
       </c>
       <c r="C95" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D95">
         <v>12</v>
       </c>
-      <c r="E95">
+      <c r="E95" s="2">
         <v>3.32</v>
       </c>
-      <c r="F95">
+      <c r="F95" s="2">
         <v>2.46</v>
       </c>
-      <c r="G95">
+      <c r="G95" s="2">
         <v>33.200000000000003</v>
       </c>
-      <c r="H95">
+      <c r="H95" s="2">
         <v>24.6</v>
       </c>
-      <c r="J95" s="1">
+      <c r="J95" s="2">
         <v>44069</v>
       </c>
-      <c r="K95" s="1">
+      <c r="K95" s="2">
         <v>44251</v>
       </c>
       <c r="L95">
@@ -4795,9 +4474,6 @@
       </c>
       <c r="N95">
         <v>2</v>
-      </c>
-      <c r="O95" t="s">
-        <v>17</v>
       </c>
       <c r="P95">
         <v>26</v>
@@ -4811,27 +4487,27 @@
         <v>2</v>
       </c>
       <c r="C96" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D96">
         <v>12</v>
       </c>
-      <c r="E96">
+      <c r="E96" s="2">
         <v>3.74</v>
       </c>
-      <c r="F96">
+      <c r="F96" s="2">
         <v>2.99</v>
       </c>
-      <c r="G96">
+      <c r="G96" s="2">
         <v>37.4</v>
       </c>
-      <c r="H96">
+      <c r="H96" s="2">
         <v>29.9</v>
       </c>
-      <c r="J96" s="1">
+      <c r="J96" s="2">
         <v>44243</v>
       </c>
-      <c r="K96" s="1">
+      <c r="K96" s="2">
         <v>44285</v>
       </c>
       <c r="L96">
@@ -4860,22 +4536,22 @@
       <c r="D97">
         <v>12</v>
       </c>
-      <c r="E97">
+      <c r="E97" s="2">
         <v>1.94</v>
       </c>
-      <c r="F97">
+      <c r="F97" s="2">
         <v>1.59</v>
       </c>
-      <c r="G97">
+      <c r="G97" s="2">
         <v>19.399999999999999</v>
       </c>
-      <c r="H97">
+      <c r="H97" s="2">
         <v>15.9</v>
       </c>
-      <c r="J97" s="1">
+      <c r="J97" s="2">
         <v>44139</v>
       </c>
-      <c r="K97" s="1">
+      <c r="K97" s="2">
         <v>44167</v>
       </c>
       <c r="L97">
@@ -4907,22 +4583,22 @@
       <c r="D98">
         <v>12</v>
       </c>
-      <c r="E98">
+      <c r="E98" s="2">
         <v>0.75</v>
       </c>
-      <c r="F98">
+      <c r="F98" s="2">
         <v>0.65</v>
       </c>
-      <c r="G98">
+      <c r="G98" s="2">
         <v>7.5</v>
       </c>
-      <c r="H98">
+      <c r="H98" s="2">
         <v>6.5</v>
       </c>
-      <c r="J98" s="1">
+      <c r="J98" s="2">
         <v>44281</v>
       </c>
-      <c r="K98" s="1">
+      <c r="K98" s="2">
         <v>44344</v>
       </c>
       <c r="L98">
@@ -4949,27 +4625,27 @@
         <v>4</v>
       </c>
       <c r="C99" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D99">
         <v>15</v>
       </c>
-      <c r="E99">
+      <c r="E99" s="2">
         <v>2.36</v>
       </c>
-      <c r="F99">
+      <c r="F99" s="2">
         <v>1.95</v>
       </c>
-      <c r="G99">
+      <c r="G99" s="2">
         <v>23.6</v>
       </c>
-      <c r="H99">
+      <c r="H99" s="2">
         <v>19.5</v>
       </c>
-      <c r="J99" s="1">
+      <c r="J99" s="2">
         <v>43909</v>
       </c>
-      <c r="K99" s="1">
+      <c r="K99" s="2">
         <v>43979</v>
       </c>
       <c r="L99">
@@ -5001,22 +4677,22 @@
       <c r="D100">
         <v>14</v>
       </c>
-      <c r="E100">
+      <c r="E100" s="2">
         <v>0.85</v>
       </c>
-      <c r="F100">
+      <c r="F100" s="2">
         <v>0.94</v>
       </c>
-      <c r="G100">
+      <c r="G100" s="2">
         <v>8.5</v>
       </c>
-      <c r="H100">
+      <c r="H100" s="2">
         <v>9.4</v>
       </c>
-      <c r="J100" s="1">
+      <c r="J100" s="2">
         <v>44005</v>
       </c>
-      <c r="K100" s="1">
+      <c r="K100" s="2">
         <v>44089</v>
       </c>
       <c r="L100">
@@ -5043,27 +4719,27 @@
         <v>3</v>
       </c>
       <c r="C101" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D101">
         <v>11</v>
       </c>
-      <c r="E101">
+      <c r="E101" s="2">
         <v>1.46</v>
       </c>
-      <c r="F101">
+      <c r="F101" s="2">
         <v>1.31</v>
       </c>
-      <c r="G101">
+      <c r="G101" s="2">
         <v>14.6</v>
       </c>
-      <c r="H101">
+      <c r="H101" s="2">
         <v>13.1</v>
       </c>
-      <c r="J101" s="1">
+      <c r="J101" s="2">
         <v>44273</v>
       </c>
-      <c r="K101" s="1">
+      <c r="K101" s="2">
         <v>44315</v>
       </c>
       <c r="L101">
@@ -5095,22 +4771,22 @@
       <c r="D102">
         <v>16</v>
       </c>
-      <c r="E102">
+      <c r="E102" s="2">
         <v>2.21</v>
       </c>
-      <c r="F102">
+      <c r="F102" s="2">
         <v>1.77</v>
       </c>
-      <c r="G102">
+      <c r="G102" s="2">
         <v>22.1</v>
       </c>
-      <c r="H102">
+      <c r="H102" s="2">
         <v>17.7</v>
       </c>
-      <c r="J102" s="1">
+      <c r="J102" s="2">
         <v>43867</v>
       </c>
-      <c r="K102" s="1">
+      <c r="K102" s="2">
         <v>43895</v>
       </c>
       <c r="L102">
@@ -5142,22 +4818,22 @@
       <c r="D103">
         <v>13</v>
       </c>
-      <c r="E103">
+      <c r="E103" s="2">
         <v>1.06</v>
       </c>
-      <c r="F103">
+      <c r="F103" s="2">
         <v>0.88</v>
       </c>
-      <c r="G103">
+      <c r="G103" s="2">
         <v>10.6</v>
       </c>
-      <c r="H103">
+      <c r="H103" s="2">
         <v>8.8000000000000007</v>
       </c>
-      <c r="J103" s="1">
+      <c r="J103" s="2">
         <v>44315</v>
       </c>
-      <c r="K103" s="1">
+      <c r="K103" s="2">
         <v>44350</v>
       </c>
       <c r="L103">
@@ -5168,9 +4844,6 @@
       </c>
       <c r="N103">
         <v>0</v>
-      </c>
-      <c r="O103" t="s">
-        <v>17</v>
       </c>
       <c r="P103">
         <v>5</v>
@@ -5189,22 +4862,22 @@
       <c r="D104">
         <v>15</v>
       </c>
-      <c r="E104">
+      <c r="E104" s="2">
         <v>2.02</v>
       </c>
-      <c r="F104">
+      <c r="F104" s="2">
         <v>1.52</v>
       </c>
-      <c r="G104">
+      <c r="G104" s="2">
         <v>20.2</v>
       </c>
-      <c r="H104">
+      <c r="H104" s="2">
         <v>15.2</v>
       </c>
-      <c r="J104" s="1">
+      <c r="J104" s="2">
         <v>44124</v>
       </c>
-      <c r="K104" s="1">
+      <c r="K104" s="2">
         <v>44173</v>
       </c>
       <c r="L104">
@@ -5231,27 +4904,27 @@
         <v>3</v>
       </c>
       <c r="C105" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D105">
         <v>16</v>
       </c>
-      <c r="E105">
+      <c r="E105" s="2">
         <v>1.19</v>
       </c>
-      <c r="F105">
+      <c r="F105" s="2">
         <v>0.95</v>
       </c>
-      <c r="G105">
+      <c r="G105" s="2">
         <v>11.9</v>
       </c>
-      <c r="H105">
+      <c r="H105" s="2">
         <v>9.5</v>
       </c>
-      <c r="J105" s="1">
+      <c r="J105" s="2">
         <v>44007</v>
       </c>
-      <c r="K105" s="1">
+      <c r="K105" s="2">
         <v>44028</v>
       </c>
       <c r="L105">
@@ -5278,27 +4951,27 @@
         <v>4</v>
       </c>
       <c r="C106" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D106">
         <v>15</v>
       </c>
-      <c r="E106">
+      <c r="E106" s="2">
         <v>1.0900000000000001</v>
       </c>
-      <c r="F106">
+      <c r="F106" s="2">
         <v>0.84</v>
       </c>
-      <c r="G106">
+      <c r="G106" s="2">
         <v>10.9</v>
       </c>
-      <c r="H106">
+      <c r="H106" s="2">
         <v>8.4</v>
       </c>
-      <c r="J106" s="1">
+      <c r="J106" s="2">
         <v>44260</v>
       </c>
-      <c r="K106" s="1">
+      <c r="K106" s="2">
         <v>44428</v>
       </c>
       <c r="L106">
@@ -5309,9 +4982,6 @@
       </c>
       <c r="N106">
         <v>0</v>
-      </c>
-      <c r="O106" t="s">
-        <v>17</v>
       </c>
       <c r="P106">
         <v>24</v>
@@ -5330,22 +5000,22 @@
       <c r="D107">
         <v>17</v>
       </c>
-      <c r="E107">
+      <c r="E107" s="2">
         <v>1.35</v>
       </c>
-      <c r="F107">
+      <c r="F107" s="2">
         <v>0.96</v>
       </c>
-      <c r="G107">
+      <c r="G107" s="2">
         <v>13.5</v>
       </c>
-      <c r="H107">
+      <c r="H107" s="2">
         <v>9.6</v>
       </c>
-      <c r="J107" s="1">
+      <c r="J107" s="2">
         <v>44427</v>
       </c>
-      <c r="K107" s="1">
+      <c r="K107" s="2">
         <v>44483</v>
       </c>
       <c r="L107">
@@ -5356,9 +5026,6 @@
       </c>
       <c r="N107">
         <v>0</v>
-      </c>
-      <c r="O107" t="s">
-        <v>17</v>
       </c>
       <c r="P107">
         <v>8</v>
@@ -5377,22 +5044,22 @@
       <c r="D108">
         <v>12</v>
       </c>
-      <c r="E108">
+      <c r="E108" s="2">
         <v>3.19</v>
       </c>
-      <c r="F108">
+      <c r="F108" s="2">
         <v>2.5299999999999998</v>
       </c>
-      <c r="G108">
+      <c r="G108" s="2">
         <v>31.9</v>
       </c>
-      <c r="H108">
+      <c r="H108" s="2">
         <v>25.3</v>
       </c>
-      <c r="J108" s="1">
+      <c r="J108" s="2">
         <v>43991</v>
       </c>
-      <c r="K108" s="1">
+      <c r="K108" s="2">
         <v>44040</v>
       </c>
       <c r="L108">
@@ -5403,9 +5070,6 @@
       </c>
       <c r="N108">
         <v>1</v>
-      </c>
-      <c r="O108" t="s">
-        <v>17</v>
       </c>
       <c r="P108">
         <v>7</v>
@@ -5424,22 +5088,22 @@
       <c r="D109">
         <v>15</v>
       </c>
-      <c r="E109">
+      <c r="E109" s="2">
         <v>1.71</v>
       </c>
-      <c r="F109">
+      <c r="F109" s="2">
         <v>1.26</v>
       </c>
-      <c r="G109">
+      <c r="G109" s="2">
         <v>17.100000000000001</v>
       </c>
-      <c r="H109">
+      <c r="H109" s="2">
         <v>12.6</v>
       </c>
-      <c r="J109" s="1">
+      <c r="J109" s="2">
         <v>44418</v>
       </c>
-      <c r="K109" s="1">
+      <c r="K109" s="2">
         <v>44439</v>
       </c>
       <c r="L109">
@@ -5450,9 +5114,6 @@
       </c>
       <c r="N109">
         <v>1</v>
-      </c>
-      <c r="O109" t="s">
-        <v>17</v>
       </c>
       <c r="P109">
         <v>3</v>
@@ -5471,22 +5132,22 @@
       <c r="D110">
         <v>14</v>
       </c>
-      <c r="E110">
+      <c r="E110" s="2">
         <v>2.69</v>
       </c>
-      <c r="F110">
+      <c r="F110" s="2">
         <v>2.17</v>
       </c>
-      <c r="G110">
+      <c r="G110" s="2">
         <v>26.9</v>
       </c>
-      <c r="H110">
+      <c r="H110" s="2">
         <v>21.7</v>
       </c>
-      <c r="J110" s="1">
+      <c r="J110" s="2">
         <v>44307</v>
       </c>
-      <c r="K110" s="1">
+      <c r="K110" s="2">
         <v>44377</v>
       </c>
       <c r="L110">
@@ -5497,9 +5158,6 @@
       </c>
       <c r="N110">
         <v>0</v>
-      </c>
-      <c r="O110" t="s">
-        <v>17</v>
       </c>
       <c r="P110">
         <v>10</v>
@@ -5518,22 +5176,22 @@
       <c r="D111">
         <v>15</v>
       </c>
-      <c r="E111">
+      <c r="E111" s="2">
         <v>3.04</v>
       </c>
-      <c r="F111">
+      <c r="F111" s="2">
         <v>2.5099999999999998</v>
       </c>
-      <c r="G111">
+      <c r="G111" s="2">
         <v>30.4</v>
       </c>
-      <c r="H111">
+      <c r="H111" s="2">
         <v>25.1</v>
       </c>
-      <c r="J111" s="1">
+      <c r="J111" s="2">
         <v>44421</v>
       </c>
-      <c r="K111" s="1">
+      <c r="K111" s="2">
         <v>44491</v>
       </c>
       <c r="L111">
@@ -5544,9 +5202,6 @@
       </c>
       <c r="N111">
         <v>0</v>
-      </c>
-      <c r="O111" t="s">
-        <v>17</v>
       </c>
       <c r="P111">
         <v>10</v>
@@ -5565,22 +5220,22 @@
       <c r="D112">
         <v>13</v>
       </c>
-      <c r="E112">
+      <c r="E112" s="2">
         <v>1.84</v>
       </c>
-      <c r="F112">
+      <c r="F112" s="2">
         <v>1.64</v>
       </c>
-      <c r="G112">
+      <c r="G112" s="2">
         <v>18.399999999999999</v>
       </c>
-      <c r="H112">
+      <c r="H112" s="2">
         <v>16.399999999999999</v>
       </c>
-      <c r="J112" s="1">
+      <c r="J112" s="2">
         <v>44327</v>
       </c>
-      <c r="K112" s="1">
+      <c r="K112" s="2">
         <v>44404</v>
       </c>
       <c r="L112">
@@ -5591,9 +5246,6 @@
       </c>
       <c r="N112">
         <v>0</v>
-      </c>
-      <c r="O112" t="s">
-        <v>17</v>
       </c>
       <c r="P112">
         <v>11</v>
@@ -5612,22 +5264,22 @@
       <c r="D113">
         <v>13</v>
       </c>
-      <c r="E113">
+      <c r="E113" s="2">
         <v>1.35</v>
       </c>
-      <c r="F113">
+      <c r="F113" s="2">
         <v>0.96</v>
       </c>
-      <c r="G113">
+      <c r="G113" s="2">
         <v>13.5</v>
       </c>
-      <c r="H113">
+      <c r="H113" s="2">
         <v>9.6</v>
       </c>
-      <c r="J113" s="1">
+      <c r="J113" s="2">
         <v>44019</v>
       </c>
-      <c r="K113" s="1">
+      <c r="K113" s="2">
         <v>44138</v>
       </c>
       <c r="L113">
@@ -5638,9 +5290,6 @@
       </c>
       <c r="N113">
         <v>0</v>
-      </c>
-      <c r="O113" t="s">
-        <v>17</v>
       </c>
       <c r="P113">
         <v>17</v>
@@ -5654,27 +5303,27 @@
         <v>2</v>
       </c>
       <c r="C114" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D114">
         <v>13</v>
       </c>
-      <c r="E114">
+      <c r="E114" s="2">
         <v>1.45</v>
       </c>
-      <c r="F114">
+      <c r="F114" s="2">
         <v>1.32</v>
       </c>
-      <c r="G114">
+      <c r="G114" s="2">
         <v>14.5</v>
       </c>
-      <c r="H114">
+      <c r="H114" s="2">
         <v>13.2</v>
       </c>
-      <c r="J114" s="1">
+      <c r="J114" s="2">
         <v>44092</v>
       </c>
-      <c r="K114" s="1">
+      <c r="K114" s="2">
         <v>44120</v>
       </c>
       <c r="L114">
@@ -5685,9 +5334,6 @@
       </c>
       <c r="N114">
         <v>0</v>
-      </c>
-      <c r="O114" t="s">
-        <v>17</v>
       </c>
       <c r="P114">
         <v>4</v>
@@ -5706,22 +5352,22 @@
       <c r="D115">
         <v>17</v>
       </c>
-      <c r="E115">
+      <c r="E115" s="2">
         <v>2.2000000000000002</v>
       </c>
-      <c r="F115">
+      <c r="F115" s="2">
         <v>1.93</v>
       </c>
-      <c r="G115">
+      <c r="G115" s="2">
         <v>22</v>
       </c>
-      <c r="H115">
+      <c r="H115" s="2">
         <v>19.3</v>
       </c>
-      <c r="J115" s="1">
+      <c r="J115" s="2">
         <v>44040</v>
       </c>
-      <c r="K115" s="1">
+      <c r="K115" s="2">
         <v>44082</v>
       </c>
       <c r="L115">
@@ -5753,22 +5399,22 @@
       <c r="D116">
         <v>13</v>
       </c>
-      <c r="E116">
+      <c r="E116" s="2">
         <v>1.81</v>
       </c>
-      <c r="F116">
+      <c r="F116" s="2">
         <v>1.43</v>
       </c>
-      <c r="G116">
+      <c r="G116" s="2">
         <v>18.100000000000001</v>
       </c>
-      <c r="H116">
+      <c r="H116" s="2">
         <v>14.3</v>
       </c>
-      <c r="J116" s="1">
+      <c r="J116" s="2">
         <v>44189</v>
       </c>
-      <c r="K116" s="1">
+      <c r="K116" s="2">
         <v>44238</v>
       </c>
       <c r="L116">
@@ -5779,9 +5425,6 @@
       </c>
       <c r="N116">
         <v>1</v>
-      </c>
-      <c r="O116" t="s">
-        <v>17</v>
       </c>
       <c r="P116">
         <v>7</v>

</xml_diff>

<commit_message>
YP-CORE_2_scores: updated handling of xlsx files and new xlsx example file
</commit_message>
<xml_diff>
--- a/docs/YP-CORE/YPwide2.xlsx
+++ b/docs/YP-CORE/YPwide2.xlsx
@@ -8,24 +8,115 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Current_share\Current_Data\MyR\shiny.psyctc.org\docs\YP-CORE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6458EE3-5BA9-4EC5-9F62-33CB090D018E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA2A4662-85B9-4169-B261-35014B332EA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14535" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="13125" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="YPwide2" sheetId="1" r:id="rId1"/>
+    <sheet name="Introduction" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="58">
+  <si>
+    <t>Introduction</t>
+  </si>
+  <si>
+    <t>The next worksheet (Data) you will find artificial data that illustrates how you can put your data in.</t>
+  </si>
+  <si>
+    <t>Try submitting this file with that data to the app and playing with it to get the hang of what the app will give you, then just delete the data in that worksheet and input your own data.</t>
+  </si>
+  <si>
+    <t>The columns you must retain in the Data worksheet are:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   RespondentID: any characters or numbers that uniquely identify the respondent (for obvious reasons of confidentiality, don’t use anything recognisable)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   TherapistID: same as for respondents/clients above</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Gender: I suggest ‘f’, ‘m’ and whatever you need if going non-binary.  The app will convert to upper case and recognises ‘F’, ‘M’ and ‘O’ but will use any other single character (or number)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Age: two digits, depending on the referential data for  CSC and RCI you use the app may use down to single year ages and between 11 and 18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   YPmean1: first YP-CORE score using mean scoring, must be between 0 and 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   YPmean2: second score, mean scoring</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   YPclin1: first YP-CORE, ‘clinical’ scoring so must be between 0 and 40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   YPclin2: second score, ‘clinical’ scoring</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Comment: enter any comment you want, the app doesn’t uses it but will export it in the analysed data it offers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Start_date: date of first score in DD/MM/YYYY format</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   End_date: date of second score, DD/MM/YYYY format</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   nSessionsAttended: what it says, presumably between 1 and many but you can use 0 to indicate someone who didn’t attend at all if you want them in your data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   nSessionsDNAed: what it says</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   nSessionsCancelled: count of sessions cancelled by the client:, nSessionsAttended + nSessionsDNAed + nSessionsCancelled = number of sessions offered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   nSessionsLate: what it says, probably a crude but useful indicator of the client’s ambivalence, resistance or frank real difficulties in attending</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   nWeeks: what it says, if you leave it blank the app will work it out from the dates</t>
+  </si>
+  <si>
+    <t>You can use as many or as few of those as you need but you must retain the columns (obviously, if you have no data the app can’t tell you much!)</t>
+  </si>
+  <si>
+    <t>You can also add as many other columns/variables to the right of those as you want, they will be exported in the analysed dataset the app offers.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At the moment they are ignored by the app but I don’t rule out adding the option to analyse things by these variables one day. </t>
+  </si>
+  <si>
+    <t>Make sure you use the first row of the worksheet to give those variables names and I recommend not having spaces in those names, so, for example:</t>
+  </si>
+  <si>
+    <t>family_size” not ‘family size’</t>
+  </si>
+  <si>
+    <t>Some of these prespecified variables have some error trapping built in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Start_date must be a valid date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   End_date must be a valid date and later than Start_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   nSessions variables must be zero or positive</t>
+  </si>
+  <si>
+    <t>Many of the cells will also colour pale red if empty</t>
+  </si>
   <si>
     <t>RespondentID</t>
   </si>
@@ -107,13 +198,33 @@
   <si>
     <t>M</t>
   </si>
+  <si>
+    <t>This spreadsheet is intended to make it easy to upload your own data from the YP-CORE (https://www.coresystemtrust.org.uk/home/instruments/yp-core-information/) to my shiny app: https://shiny.psyctc.org/apps/YP-CORE_2_scores/ which will process one or two YP-CORE scores per row/person.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -139,18 +250,161 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FFCC0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCCC"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFCC0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCCC"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFCC0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCCC"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFCC0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCCC"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFCC0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCCC"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFCC0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCCC"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -272,10 +526,193 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:B36"/>
+  <sheetViews>
+    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="189.140625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="11.5703125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B3" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B16" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B27" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B28" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B29" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B30" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B32" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B33" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B34" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B35" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B36" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P116"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <pane xSplit="1830" ySplit="555" topLeftCell="B1" activePane="bottomRight"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -284,11 +721,11 @@
     <col min="2" max="2" width="10.85546875" customWidth="1"/>
     <col min="3" max="3" width="7.42578125" customWidth="1"/>
     <col min="4" max="4" width="4.7109375" customWidth="1"/>
-    <col min="5" max="6" width="9.42578125" style="2" customWidth="1"/>
-    <col min="7" max="8" width="7.85546875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="63" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" style="2" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" style="2" customWidth="1"/>
+    <col min="5" max="6" width="9.42578125" customWidth="1"/>
+    <col min="7" max="8" width="7.85546875" customWidth="1"/>
+    <col min="9" max="9" width="63" style="3" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" style="4" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" style="4" customWidth="1"/>
     <col min="12" max="12" width="17.28515625" customWidth="1"/>
     <col min="13" max="13" width="15.7109375" customWidth="1"/>
     <col min="14" max="14" width="18" customWidth="1"/>
@@ -296,54 +733,54 @@
     <col min="16" max="16" width="8.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
+    <row r="1" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
@@ -354,24 +791,24 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D2">
         <v>11</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2">
         <v>1.62</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2">
         <v>1.1299999999999999</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2">
         <v>16.2</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="2">
+      <c r="I2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2" s="4">
         <v>43924</v>
       </c>
       <c r="L2">
@@ -398,24 +835,24 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D3">
         <v>11</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3">
         <v>2.2599999999999998</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3">
         <v>1.76</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3">
         <v>17.600000000000001</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" s="2">
+      <c r="I3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" s="4">
         <v>43931</v>
       </c>
       <c r="L3">
@@ -442,27 +879,27 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D4">
         <v>12</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4">
         <v>1.9</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4">
         <v>1.47</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4">
         <v>19</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4">
         <v>14.7</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" s="2">
+      <c r="I4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J4" s="4">
         <v>43915</v>
       </c>
       <c r="L4">
@@ -486,24 +923,24 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D5">
         <v>13</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5">
         <v>1.32</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5">
         <v>17.399999999999999</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5">
         <v>13.2</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5" s="2">
+      <c r="I5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J5" s="4">
         <v>44097</v>
       </c>
       <c r="L5">
@@ -527,15 +964,15 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D6">
         <v>14</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J6" s="2">
+      <c r="I6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="J6" s="4">
         <v>44411</v>
       </c>
       <c r="L6">
@@ -562,21 +999,21 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D7">
         <v>15</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7">
         <v>5</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7">
         <v>2.0099999999999998</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J7" s="2">
+      <c r="I7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J7" s="4">
         <v>44174</v>
       </c>
       <c r="L7">
@@ -603,21 +1040,21 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D8">
         <v>16</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8">
         <v>-1</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8">
         <v>2.92</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J8" s="2">
+      <c r="I8" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J8" s="4">
         <v>44421</v>
       </c>
       <c r="L8">
@@ -644,21 +1081,21 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D9">
         <v>17</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9">
         <v>56</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9">
         <v>22.6</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J9" s="2">
+      <c r="I9" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J9" s="4">
         <v>44036</v>
       </c>
       <c r="L9">
@@ -685,21 +1122,21 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D10">
         <v>18</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10">
         <v>-1</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10">
         <v>14.3</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J10" s="2">
+      <c r="I10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J10" s="4">
         <v>44167</v>
       </c>
       <c r="L10">
@@ -726,27 +1163,27 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="D11">
         <v>11</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11">
         <v>1.62</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11">
         <v>1.2</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11">
         <v>16.2</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11">
         <v>12</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J11" s="2">
+      <c r="I11" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J11" s="4">
         <v>44033</v>
       </c>
       <c r="L11">
@@ -772,22 +1209,22 @@
       <c r="D12">
         <v>11</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12">
         <v>1.62</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12">
         <v>1.2</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12">
         <v>16.2</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12">
         <v>12</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J12" s="2">
+      <c r="I12" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J12" s="4">
         <v>44147</v>
       </c>
       <c r="L12">
@@ -814,27 +1251,27 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="D13">
         <v>11</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13">
         <v>1.62</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13">
         <v>1.2</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13">
         <v>16.2</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13">
         <v>12</v>
       </c>
-      <c r="I13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J13" s="2">
+      <c r="I13" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="J13" s="4">
         <v>43868</v>
       </c>
       <c r="L13">
@@ -855,24 +1292,24 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="2">
+        <v>46</v>
+      </c>
+      <c r="E14">
         <v>3.87</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14">
         <v>3.15</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14">
         <v>38.700000000000003</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14">
         <v>31.5</v>
       </c>
-      <c r="I14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J14" s="2">
+      <c r="I14" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J14" s="4">
         <v>44393</v>
       </c>
       <c r="L14">
@@ -893,24 +1330,24 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D15">
         <v>10</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15">
         <v>3.87</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15">
         <v>3.15</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15">
         <v>38.700000000000003</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15">
         <v>31.5</v>
       </c>
-      <c r="J15" s="2">
+      <c r="J15" s="4">
         <v>44434</v>
       </c>
       <c r="L15">
@@ -931,24 +1368,24 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D16">
         <v>12</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16">
         <v>3.87</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16">
         <v>3.15</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16">
         <v>38.700000000000003</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16">
         <v>31.5</v>
       </c>
-      <c r="J16" s="2">
+      <c r="J16" s="4">
         <v>44204</v>
       </c>
       <c r="L16">
@@ -974,7 +1411,7 @@
       <c r="B17">
         <v>1</v>
       </c>
-      <c r="J17" s="2">
+      <c r="J17" s="4">
         <v>43858</v>
       </c>
       <c r="L17">
@@ -998,24 +1435,24 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D18">
         <v>11</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18">
         <v>1.62</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18">
         <v>1.2</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18">
         <v>16.2</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H18">
         <v>12</v>
       </c>
-      <c r="J18" s="2">
+      <c r="J18" s="4">
         <v>44413</v>
       </c>
       <c r="L18">
@@ -1042,24 +1479,24 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D19">
         <v>12</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19">
         <v>3.87</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19">
         <v>3.15</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G19">
         <v>38.700000000000003</v>
       </c>
-      <c r="H19" s="2">
+      <c r="H19">
         <v>31.5</v>
       </c>
-      <c r="J19" s="2">
+      <c r="J19" s="4">
         <v>44084</v>
       </c>
       <c r="L19">
@@ -1083,24 +1520,24 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D20">
         <v>12</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20">
         <v>2.42</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20">
         <v>1.79</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20">
         <v>24.2</v>
       </c>
-      <c r="H20" s="2">
+      <c r="H20">
         <v>17.899999999999999</v>
       </c>
-      <c r="J20" s="2">
+      <c r="J20" s="4">
         <v>44133</v>
       </c>
       <c r="L20">
@@ -1127,24 +1564,24 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D21">
         <v>13</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21">
         <v>2.1800000000000002</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21">
         <v>1.75</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G21">
         <v>21.8</v>
       </c>
-      <c r="H21" s="2">
+      <c r="H21">
         <v>17.5</v>
       </c>
-      <c r="J21" s="2">
+      <c r="J21" s="4">
         <v>44470</v>
       </c>
       <c r="L21">
@@ -1171,24 +1608,24 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D22">
         <v>13</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22">
         <v>2.62</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22">
         <v>2.09</v>
       </c>
-      <c r="G22" s="2">
+      <c r="G22">
         <v>26.2</v>
       </c>
-      <c r="H22" s="2">
+      <c r="H22">
         <v>20.9</v>
       </c>
-      <c r="J22" s="2">
+      <c r="J22" s="4">
         <v>44040</v>
       </c>
       <c r="L22">
@@ -1212,24 +1649,24 @@
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D23">
         <v>14</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23">
         <v>1.27</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F23">
         <v>1.1000000000000001</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G23">
         <v>12.7</v>
       </c>
-      <c r="H23" s="2">
+      <c r="H23">
         <v>11</v>
       </c>
-      <c r="J23" s="2">
+      <c r="J23" s="4">
         <v>44168</v>
       </c>
       <c r="L23">
@@ -1256,24 +1693,24 @@
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D24">
         <v>14</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24">
         <v>3.02</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F24">
         <v>2.38</v>
       </c>
-      <c r="G24" s="2">
+      <c r="G24">
         <v>30.2</v>
       </c>
-      <c r="H24" s="2">
+      <c r="H24">
         <v>23.8</v>
       </c>
-      <c r="J24" s="2">
+      <c r="J24" s="4">
         <v>44069</v>
       </c>
       <c r="L24">
@@ -1297,24 +1734,24 @@
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D25">
         <v>15</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25">
         <v>2.75</v>
       </c>
-      <c r="F25" s="2">
+      <c r="F25">
         <v>2.23</v>
       </c>
-      <c r="G25" s="2">
+      <c r="G25">
         <v>27.5</v>
       </c>
-      <c r="H25" s="2">
+      <c r="H25">
         <v>22.3</v>
       </c>
-      <c r="J25" s="2">
+      <c r="J25" s="4">
         <v>44418</v>
       </c>
       <c r="L25">
@@ -1338,24 +1775,24 @@
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D26">
         <v>15</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E26">
         <v>1.24</v>
       </c>
-      <c r="F26" s="2">
+      <c r="F26">
         <v>1.08</v>
       </c>
-      <c r="G26" s="2">
+      <c r="G26">
         <v>12.4</v>
       </c>
-      <c r="H26" s="2">
+      <c r="H26">
         <v>10.8</v>
       </c>
-      <c r="J26" s="2">
+      <c r="J26" s="4">
         <v>44194</v>
       </c>
       <c r="L26">
@@ -1379,24 +1816,24 @@
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D27">
         <v>16</v>
       </c>
-      <c r="E27" s="2">
+      <c r="E27">
         <v>1.4</v>
       </c>
-      <c r="F27" s="2">
+      <c r="F27">
         <v>1.05</v>
       </c>
-      <c r="G27" s="2">
+      <c r="G27">
         <v>14</v>
       </c>
-      <c r="H27" s="2">
+      <c r="H27">
         <v>10.5</v>
       </c>
-      <c r="J27" s="2">
+      <c r="J27" s="4">
         <v>44020</v>
       </c>
       <c r="L27">
@@ -1420,24 +1857,24 @@
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D28">
         <v>16</v>
       </c>
-      <c r="E28" s="2">
+      <c r="E28">
         <v>2.4700000000000002</v>
       </c>
-      <c r="F28" s="2">
+      <c r="F28">
         <v>1.99</v>
       </c>
-      <c r="G28" s="2">
+      <c r="G28">
         <v>24.7</v>
       </c>
-      <c r="H28" s="2">
+      <c r="H28">
         <v>19.899999999999999</v>
       </c>
-      <c r="J28" s="2">
+      <c r="J28" s="4">
         <v>43887</v>
       </c>
       <c r="L28">
@@ -1464,24 +1901,24 @@
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D29">
         <v>17</v>
       </c>
-      <c r="E29" s="2">
+      <c r="E29">
         <v>1.28</v>
       </c>
-      <c r="F29" s="2">
+      <c r="F29">
         <v>0.92</v>
       </c>
-      <c r="G29" s="2">
+      <c r="G29">
         <v>12.8</v>
       </c>
-      <c r="H29" s="2">
+      <c r="H29">
         <v>9.1999999999999993</v>
       </c>
-      <c r="J29" s="2">
+      <c r="J29" s="4">
         <v>44159</v>
       </c>
       <c r="L29">
@@ -1505,24 +1942,24 @@
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D30">
         <v>17</v>
       </c>
-      <c r="E30" s="2">
+      <c r="E30">
         <v>3.17</v>
       </c>
-      <c r="F30" s="2">
+      <c r="F30">
         <v>2.74</v>
       </c>
-      <c r="G30" s="2">
+      <c r="G30">
         <v>31.7</v>
       </c>
-      <c r="H30" s="2">
+      <c r="H30">
         <v>27.4</v>
       </c>
-      <c r="J30" s="2">
+      <c r="J30" s="4">
         <v>44244</v>
       </c>
       <c r="L30">
@@ -1549,24 +1986,24 @@
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D31">
         <v>18</v>
       </c>
-      <c r="E31" s="2">
+      <c r="E31">
         <v>1.82</v>
       </c>
-      <c r="F31" s="2">
+      <c r="F31">
         <v>1.44</v>
       </c>
-      <c r="G31" s="2">
+      <c r="G31">
         <v>18.2</v>
       </c>
-      <c r="H31" s="2">
+      <c r="H31">
         <v>14.4</v>
       </c>
-      <c r="J31" s="2">
+      <c r="J31" s="4">
         <v>44236</v>
       </c>
       <c r="L31">
@@ -1593,24 +2030,24 @@
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D32">
         <v>18</v>
       </c>
-      <c r="E32" s="2">
+      <c r="E32">
         <v>2.95</v>
       </c>
-      <c r="F32" s="2">
+      <c r="F32">
         <v>2.38</v>
       </c>
-      <c r="G32" s="2">
+      <c r="G32">
         <v>29.5</v>
       </c>
-      <c r="H32" s="2">
+      <c r="H32">
         <v>23.8</v>
       </c>
-      <c r="J32" s="2">
+      <c r="J32" s="4">
         <v>44047</v>
       </c>
       <c r="L32">
@@ -1637,27 +2074,27 @@
         <v>2</v>
       </c>
       <c r="C33" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D33">
         <v>13</v>
       </c>
-      <c r="E33" s="2">
+      <c r="E33">
         <v>1.53</v>
       </c>
-      <c r="F33" s="2">
+      <c r="F33">
         <v>1.31</v>
       </c>
-      <c r="G33" s="2">
+      <c r="G33">
         <v>15.3</v>
       </c>
-      <c r="H33" s="2">
+      <c r="H33">
         <v>13.1</v>
       </c>
-      <c r="J33" s="2">
+      <c r="J33" s="4">
         <v>44124</v>
       </c>
-      <c r="K33" s="2">
+      <c r="K33" s="4">
         <v>44173</v>
       </c>
       <c r="L33">
@@ -1681,27 +2118,27 @@
         <v>2</v>
       </c>
       <c r="C34" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D34">
         <v>15</v>
       </c>
-      <c r="E34" s="2">
+      <c r="E34">
         <v>2.4</v>
       </c>
-      <c r="F34" s="2">
+      <c r="F34">
         <v>1.73</v>
       </c>
-      <c r="G34" s="2">
+      <c r="G34">
         <v>24</v>
       </c>
-      <c r="H34" s="2">
+      <c r="H34">
         <v>17.3</v>
       </c>
-      <c r="J34" s="2">
+      <c r="J34" s="4">
         <v>43935</v>
       </c>
-      <c r="K34" s="2">
+      <c r="K34" s="4">
         <v>43991</v>
       </c>
       <c r="L34">
@@ -1725,27 +2162,27 @@
         <v>5</v>
       </c>
       <c r="C35" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D35">
         <v>18</v>
       </c>
-      <c r="E35" s="2">
+      <c r="E35">
         <v>2.25</v>
       </c>
-      <c r="F35" s="2">
+      <c r="F35">
         <v>1.73</v>
       </c>
-      <c r="G35" s="2">
+      <c r="G35">
         <v>22.5</v>
       </c>
-      <c r="H35" s="2">
+      <c r="H35">
         <v>17.3</v>
       </c>
-      <c r="J35" s="2">
+      <c r="J35" s="4">
         <v>44127</v>
       </c>
-      <c r="K35" s="2">
+      <c r="K35" s="4">
         <v>44211</v>
       </c>
       <c r="L35">
@@ -1772,27 +2209,27 @@
         <v>2</v>
       </c>
       <c r="C36" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D36">
         <v>16</v>
       </c>
-      <c r="E36" s="2">
+      <c r="E36">
         <v>2.29</v>
       </c>
-      <c r="F36" s="2">
+      <c r="F36">
         <v>2.04</v>
       </c>
-      <c r="G36" s="2">
+      <c r="G36">
         <v>22.9</v>
       </c>
-      <c r="H36" s="2">
+      <c r="H36">
         <v>20.399999999999999</v>
       </c>
-      <c r="J36" s="2">
+      <c r="J36" s="4">
         <v>43893</v>
       </c>
-      <c r="K36" s="2">
+      <c r="K36" s="4">
         <v>43914</v>
       </c>
       <c r="L36">
@@ -1819,27 +2256,27 @@
         <v>4</v>
       </c>
       <c r="C37" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D37">
         <v>15</v>
       </c>
-      <c r="E37" s="2">
+      <c r="E37">
         <v>1.62</v>
       </c>
-      <c r="F37" s="2">
+      <c r="F37">
         <v>1.44</v>
       </c>
-      <c r="G37" s="2">
+      <c r="G37">
         <v>16.2</v>
       </c>
-      <c r="H37" s="2">
+      <c r="H37">
         <v>14.4</v>
       </c>
-      <c r="J37" s="2">
+      <c r="J37" s="4">
         <v>44238</v>
       </c>
-      <c r="K37" s="2">
+      <c r="K37" s="4">
         <v>44322</v>
       </c>
       <c r="L37">
@@ -1863,27 +2300,27 @@
         <v>5</v>
       </c>
       <c r="C38" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D38">
         <v>17</v>
       </c>
-      <c r="E38" s="2">
+      <c r="E38">
         <v>2.34</v>
       </c>
-      <c r="F38" s="2">
+      <c r="F38">
         <v>1.85</v>
       </c>
-      <c r="G38" s="2">
+      <c r="G38">
         <v>23.4</v>
       </c>
-      <c r="H38" s="2">
+      <c r="H38">
         <v>18.5</v>
       </c>
-      <c r="J38" s="2">
+      <c r="J38" s="4">
         <v>44166</v>
       </c>
-      <c r="K38" s="2">
+      <c r="K38" s="4">
         <v>44215</v>
       </c>
       <c r="L38">
@@ -1907,27 +2344,27 @@
         <v>5</v>
       </c>
       <c r="C39" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D39">
         <v>14</v>
       </c>
-      <c r="E39" s="2">
+      <c r="E39">
         <v>2.42</v>
       </c>
-      <c r="F39" s="2">
+      <c r="F39">
         <v>1.9</v>
       </c>
-      <c r="G39" s="2">
+      <c r="G39">
         <v>24.2</v>
       </c>
-      <c r="H39" s="2">
+      <c r="H39">
         <v>19</v>
       </c>
-      <c r="J39" s="2">
+      <c r="J39" s="4">
         <v>44125</v>
       </c>
-      <c r="K39" s="2">
+      <c r="K39" s="4">
         <v>44188</v>
       </c>
       <c r="L39">
@@ -1951,27 +2388,27 @@
         <v>5</v>
       </c>
       <c r="C40" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D40">
         <v>13</v>
       </c>
-      <c r="E40" s="2">
+      <c r="E40">
         <v>2.81</v>
       </c>
-      <c r="F40" s="2">
+      <c r="F40">
         <v>2.34</v>
       </c>
-      <c r="G40" s="2">
+      <c r="G40">
         <v>28.1</v>
       </c>
-      <c r="H40" s="2">
+      <c r="H40">
         <v>23.4</v>
       </c>
-      <c r="J40" s="2">
+      <c r="J40" s="4">
         <v>44440</v>
       </c>
-      <c r="K40" s="2">
+      <c r="K40" s="4">
         <v>44482</v>
       </c>
       <c r="L40">
@@ -1995,27 +2432,27 @@
         <v>3</v>
       </c>
       <c r="C41" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D41">
         <v>13</v>
       </c>
-      <c r="E41" s="2">
+      <c r="E41">
         <v>2.06</v>
       </c>
-      <c r="F41" s="2">
+      <c r="F41">
         <v>1.62</v>
       </c>
-      <c r="G41" s="2">
+      <c r="G41">
         <v>20.6</v>
       </c>
-      <c r="H41" s="2">
+      <c r="H41">
         <v>16.2</v>
       </c>
-      <c r="J41" s="2">
+      <c r="J41" s="4">
         <v>43852</v>
       </c>
-      <c r="K41" s="2">
+      <c r="K41" s="4">
         <v>43915</v>
       </c>
       <c r="L41">
@@ -2042,27 +2479,27 @@
         <v>5</v>
       </c>
       <c r="C42" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D42">
         <v>15</v>
       </c>
-      <c r="E42" s="2">
+      <c r="E42">
         <v>1.94</v>
       </c>
-      <c r="F42" s="2">
+      <c r="F42">
         <v>1.53</v>
       </c>
-      <c r="G42" s="2">
+      <c r="G42">
         <v>19.399999999999999</v>
       </c>
-      <c r="H42" s="2">
+      <c r="H42">
         <v>15.3</v>
       </c>
-      <c r="J42" s="2">
+      <c r="J42" s="4">
         <v>44209</v>
       </c>
-      <c r="K42" s="2">
+      <c r="K42" s="4">
         <v>44244</v>
       </c>
       <c r="L42">
@@ -2089,27 +2526,27 @@
         <v>4</v>
       </c>
       <c r="C43" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D43">
         <v>16</v>
       </c>
-      <c r="E43" s="2">
+      <c r="E43">
         <v>2.71</v>
       </c>
-      <c r="F43" s="2">
+      <c r="F43">
         <v>2.35</v>
       </c>
-      <c r="G43" s="2">
+      <c r="G43">
         <v>27.1</v>
       </c>
-      <c r="H43" s="2">
+      <c r="H43">
         <v>23.5</v>
       </c>
-      <c r="J43" s="2">
+      <c r="J43" s="4">
         <v>44287</v>
       </c>
-      <c r="K43" s="2">
+      <c r="K43" s="4">
         <v>44350</v>
       </c>
       <c r="L43">
@@ -2136,27 +2573,27 @@
         <v>3</v>
       </c>
       <c r="C44" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D44">
         <v>15</v>
       </c>
-      <c r="E44" s="2">
+      <c r="E44">
         <v>2.11</v>
       </c>
-      <c r="F44" s="2">
+      <c r="F44">
         <v>1.81</v>
       </c>
-      <c r="G44" s="2">
+      <c r="G44">
         <v>21.1</v>
       </c>
-      <c r="H44" s="2">
+      <c r="H44">
         <v>18.100000000000001</v>
       </c>
-      <c r="J44" s="2">
+      <c r="J44" s="4">
         <v>44125</v>
       </c>
-      <c r="K44" s="2">
+      <c r="K44" s="4">
         <v>44174</v>
       </c>
       <c r="L44">
@@ -2183,27 +2620,27 @@
         <v>2</v>
       </c>
       <c r="C45" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D45">
         <v>14</v>
       </c>
-      <c r="E45" s="2">
+      <c r="E45">
         <v>2.4300000000000002</v>
       </c>
-      <c r="F45" s="2">
+      <c r="F45">
         <v>2.08</v>
       </c>
-      <c r="G45" s="2">
+      <c r="G45">
         <v>24.3</v>
       </c>
-      <c r="H45" s="2">
+      <c r="H45">
         <v>20.8</v>
       </c>
-      <c r="J45" s="2">
+      <c r="J45" s="4">
         <v>44442</v>
       </c>
-      <c r="K45" s="2">
+      <c r="K45" s="4">
         <v>44477</v>
       </c>
       <c r="L45">
@@ -2230,27 +2667,27 @@
         <v>4</v>
       </c>
       <c r="C46" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D46">
         <v>15</v>
       </c>
-      <c r="E46" s="2">
+      <c r="E46">
         <v>0.92</v>
       </c>
-      <c r="F46" s="2">
+      <c r="F46">
         <v>0.68</v>
       </c>
-      <c r="G46" s="2">
+      <c r="G46">
         <v>9.1999999999999993</v>
       </c>
-      <c r="H46" s="2">
+      <c r="H46">
         <v>6.8</v>
       </c>
-      <c r="J46" s="2">
+      <c r="J46" s="4">
         <v>44251</v>
       </c>
-      <c r="K46" s="2">
+      <c r="K46" s="4">
         <v>44286</v>
       </c>
       <c r="L46">
@@ -2274,27 +2711,27 @@
         <v>3</v>
       </c>
       <c r="C47" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D47">
         <v>16</v>
       </c>
-      <c r="E47" s="2">
+      <c r="E47">
         <v>1.39</v>
       </c>
-      <c r="F47" s="2">
+      <c r="F47">
         <v>1.01</v>
       </c>
-      <c r="G47" s="2">
+      <c r="G47">
         <v>13.9</v>
       </c>
-      <c r="H47" s="2">
+      <c r="H47">
         <v>10.1</v>
       </c>
-      <c r="J47" s="2">
+      <c r="J47" s="4">
         <v>44469</v>
       </c>
-      <c r="K47" s="2">
+      <c r="K47" s="4">
         <v>44546</v>
       </c>
       <c r="L47">
@@ -2323,22 +2760,22 @@
       <c r="D48">
         <v>15</v>
       </c>
-      <c r="E48" s="2">
+      <c r="E48">
         <v>2.87</v>
       </c>
-      <c r="F48" s="2">
+      <c r="F48">
         <v>2.44</v>
       </c>
-      <c r="G48" s="2">
+      <c r="G48">
         <v>28.7</v>
       </c>
-      <c r="H48" s="2">
+      <c r="H48">
         <v>24.4</v>
       </c>
-      <c r="J48" s="2">
+      <c r="J48" s="4">
         <v>43846</v>
       </c>
-      <c r="K48" s="2">
+      <c r="K48" s="4">
         <v>43860</v>
       </c>
       <c r="L48">
@@ -2365,27 +2802,27 @@
         <v>2</v>
       </c>
       <c r="C49" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D49">
         <v>14</v>
       </c>
-      <c r="E49" s="2">
+      <c r="E49">
         <v>2.0699999999999998</v>
       </c>
-      <c r="F49" s="2">
+      <c r="F49">
         <v>1.67</v>
       </c>
-      <c r="G49" s="2">
+      <c r="G49">
         <v>20.7</v>
       </c>
-      <c r="H49" s="2">
+      <c r="H49">
         <v>16.7</v>
       </c>
-      <c r="J49" s="2">
+      <c r="J49" s="4">
         <v>44182</v>
       </c>
-      <c r="K49" s="2">
+      <c r="K49" s="4">
         <v>44203</v>
       </c>
       <c r="L49">
@@ -2409,27 +2846,27 @@
         <v>3</v>
       </c>
       <c r="C50" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D50">
         <v>17</v>
       </c>
-      <c r="E50" s="2">
+      <c r="E50">
         <v>1.48</v>
       </c>
-      <c r="F50" s="2">
+      <c r="F50">
         <v>1.26</v>
       </c>
-      <c r="G50" s="2">
+      <c r="G50">
         <v>14.8</v>
       </c>
-      <c r="H50" s="2">
+      <c r="H50">
         <v>12.6</v>
       </c>
-      <c r="J50" s="2">
+      <c r="J50" s="4">
         <v>44232</v>
       </c>
-      <c r="K50" s="2">
+      <c r="K50" s="4">
         <v>44274</v>
       </c>
       <c r="L50">
@@ -2453,27 +2890,27 @@
         <v>4</v>
       </c>
       <c r="C51" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D51">
         <v>18</v>
       </c>
-      <c r="E51" s="2">
+      <c r="E51">
         <v>0.72</v>
       </c>
-      <c r="F51" s="2">
+      <c r="F51">
         <v>0.65</v>
       </c>
-      <c r="G51" s="2">
+      <c r="G51">
         <v>7.2</v>
       </c>
-      <c r="H51" s="2">
+      <c r="H51">
         <v>6.5</v>
       </c>
-      <c r="J51" s="2">
+      <c r="J51" s="4">
         <v>44113</v>
       </c>
-      <c r="K51" s="2">
+      <c r="K51" s="4">
         <v>44141</v>
       </c>
       <c r="L51">
@@ -2500,27 +2937,27 @@
         <v>5</v>
       </c>
       <c r="C52" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D52">
         <v>13</v>
       </c>
-      <c r="E52" s="2">
+      <c r="E52">
         <v>0.99</v>
       </c>
-      <c r="F52" s="2">
+      <c r="F52">
         <v>0.7</v>
       </c>
-      <c r="G52" s="2">
+      <c r="G52">
         <v>9.9</v>
       </c>
-      <c r="H52" s="2">
+      <c r="H52">
         <v>7</v>
       </c>
-      <c r="J52" s="2">
+      <c r="J52" s="4">
         <v>44461</v>
       </c>
-      <c r="K52" s="2">
+      <c r="K52" s="4">
         <v>44482</v>
       </c>
       <c r="L52">
@@ -2544,27 +2981,27 @@
         <v>3</v>
       </c>
       <c r="C53" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D53">
         <v>15</v>
       </c>
-      <c r="E53" s="2">
+      <c r="E53">
         <v>2.0099999999999998</v>
       </c>
-      <c r="F53" s="2">
+      <c r="F53">
         <v>1.51</v>
       </c>
-      <c r="G53" s="2">
+      <c r="G53">
         <v>20.100000000000001</v>
       </c>
-      <c r="H53" s="2">
+      <c r="H53">
         <v>15.1</v>
       </c>
-      <c r="J53" s="2">
+      <c r="J53" s="4">
         <v>44209</v>
       </c>
-      <c r="K53" s="2">
+      <c r="K53" s="4">
         <v>44321</v>
       </c>
       <c r="L53">
@@ -2591,27 +3028,27 @@
         <v>5</v>
       </c>
       <c r="C54" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D54">
         <v>11</v>
       </c>
-      <c r="E54" s="2">
+      <c r="E54">
         <v>3.09</v>
       </c>
-      <c r="F54" s="2">
+      <c r="F54">
         <v>2.68</v>
       </c>
-      <c r="G54" s="2">
+      <c r="G54">
         <v>30.9</v>
       </c>
-      <c r="H54" s="2">
+      <c r="H54">
         <v>26.8</v>
       </c>
-      <c r="J54" s="2">
+      <c r="J54" s="4">
         <v>44462</v>
       </c>
-      <c r="K54" s="2">
+      <c r="K54" s="4">
         <v>44483</v>
       </c>
       <c r="L54">
@@ -2635,27 +3072,27 @@
         <v>4</v>
       </c>
       <c r="C55" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D55">
         <v>17</v>
       </c>
-      <c r="E55" s="2">
+      <c r="E55">
         <v>1.99</v>
       </c>
-      <c r="F55" s="2">
+      <c r="F55">
         <v>1.59</v>
       </c>
-      <c r="G55" s="2">
+      <c r="G55">
         <v>19.899999999999999</v>
       </c>
-      <c r="H55" s="2">
+      <c r="H55">
         <v>15.9</v>
       </c>
-      <c r="J55" s="2">
+      <c r="J55" s="4">
         <v>44084</v>
       </c>
-      <c r="K55" s="2">
+      <c r="K55" s="4">
         <v>44133</v>
       </c>
       <c r="L55">
@@ -2682,27 +3119,27 @@
         <v>4</v>
       </c>
       <c r="C56" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D56">
         <v>16</v>
       </c>
-      <c r="E56" s="2">
+      <c r="E56">
         <v>1.54</v>
       </c>
-      <c r="F56" s="2">
+      <c r="F56">
         <v>1.35</v>
       </c>
-      <c r="G56" s="2">
+      <c r="G56">
         <v>15.4</v>
       </c>
-      <c r="H56" s="2">
+      <c r="H56">
         <v>13.5</v>
       </c>
-      <c r="J56" s="2">
+      <c r="J56" s="4">
         <v>44337</v>
       </c>
-      <c r="K56" s="2">
+      <c r="K56" s="4">
         <v>44421</v>
       </c>
       <c r="L56">
@@ -2729,27 +3166,27 @@
         <v>2</v>
       </c>
       <c r="C57" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D57">
         <v>17</v>
       </c>
-      <c r="E57" s="2">
+      <c r="E57">
         <v>2.11</v>
       </c>
-      <c r="F57" s="2">
+      <c r="F57">
         <v>1.53</v>
       </c>
-      <c r="G57" s="2">
+      <c r="G57">
         <v>21.1</v>
       </c>
-      <c r="H57" s="2">
+      <c r="H57">
         <v>15.3</v>
       </c>
-      <c r="J57" s="2">
+      <c r="J57" s="4">
         <v>44400</v>
       </c>
-      <c r="K57" s="2">
+      <c r="K57" s="4">
         <v>44442</v>
       </c>
       <c r="L57">
@@ -2773,27 +3210,27 @@
         <v>4</v>
       </c>
       <c r="C58" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D58">
         <v>14</v>
       </c>
-      <c r="E58" s="2">
+      <c r="E58">
         <v>2.27</v>
       </c>
-      <c r="F58" s="2">
+      <c r="F58">
         <v>1.69</v>
       </c>
-      <c r="G58" s="2">
+      <c r="G58">
         <v>22.7</v>
       </c>
-      <c r="H58" s="2">
+      <c r="H58">
         <v>16.899999999999999</v>
       </c>
-      <c r="J58" s="2">
+      <c r="J58" s="4">
         <v>44420</v>
       </c>
-      <c r="K58" s="2">
+      <c r="K58" s="4">
         <v>44441</v>
       </c>
       <c r="L58">
@@ -2820,27 +3257,27 @@
         <v>4</v>
       </c>
       <c r="C59" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D59">
         <v>15</v>
       </c>
-      <c r="E59" s="2">
+      <c r="E59">
         <v>1.31</v>
       </c>
-      <c r="F59" s="2">
+      <c r="F59">
         <v>1.22</v>
       </c>
-      <c r="G59" s="2">
+      <c r="G59">
         <v>13.1</v>
       </c>
-      <c r="H59" s="2">
+      <c r="H59">
         <v>12.2</v>
       </c>
-      <c r="J59" s="2">
+      <c r="J59" s="4">
         <v>44330</v>
       </c>
-      <c r="K59" s="2">
+      <c r="K59" s="4">
         <v>44379</v>
       </c>
       <c r="L59">
@@ -2864,27 +3301,27 @@
         <v>4</v>
       </c>
       <c r="C60" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D60">
         <v>12</v>
       </c>
-      <c r="E60" s="2">
+      <c r="E60">
         <v>0.98</v>
       </c>
-      <c r="F60" s="2">
+      <c r="F60">
         <v>0.67</v>
       </c>
-      <c r="G60" s="2">
+      <c r="G60">
         <v>9.8000000000000007</v>
       </c>
-      <c r="H60" s="2">
+      <c r="H60">
         <v>6.7</v>
       </c>
-      <c r="J60" s="2">
+      <c r="J60" s="4">
         <v>43952</v>
       </c>
-      <c r="K60" s="2">
+      <c r="K60" s="4">
         <v>44001</v>
       </c>
       <c r="L60">
@@ -2911,27 +3348,27 @@
         <v>5</v>
       </c>
       <c r="C61" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D61">
         <v>12</v>
       </c>
-      <c r="E61" s="2">
+      <c r="E61">
         <v>3.08</v>
       </c>
-      <c r="F61" s="2">
+      <c r="F61">
         <v>2.65</v>
       </c>
-      <c r="G61" s="2">
+      <c r="G61">
         <v>30.8</v>
       </c>
-      <c r="H61" s="2">
+      <c r="H61">
         <v>26.5</v>
       </c>
-      <c r="J61" s="2">
+      <c r="J61" s="4">
         <v>44092</v>
       </c>
-      <c r="K61" s="2">
+      <c r="K61" s="4">
         <v>44113</v>
       </c>
       <c r="L61">
@@ -2955,27 +3392,27 @@
         <v>5</v>
       </c>
       <c r="C62" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D62">
         <v>11</v>
       </c>
-      <c r="E62" s="2">
+      <c r="E62">
         <v>2.94</v>
       </c>
-      <c r="F62" s="2">
+      <c r="F62">
         <v>2.2999999999999998</v>
       </c>
-      <c r="G62" s="2">
+      <c r="G62">
         <v>29.4</v>
       </c>
-      <c r="H62" s="2">
+      <c r="H62">
         <v>23</v>
       </c>
-      <c r="J62" s="2">
+      <c r="J62" s="4">
         <v>43861</v>
       </c>
-      <c r="K62" s="2">
+      <c r="K62" s="4">
         <v>43875</v>
       </c>
       <c r="L62">
@@ -3002,27 +3439,27 @@
         <v>2</v>
       </c>
       <c r="C63" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D63">
         <v>14</v>
       </c>
-      <c r="E63" s="2">
+      <c r="E63">
         <v>2.2599999999999998</v>
       </c>
-      <c r="F63" s="2">
+      <c r="F63">
         <v>1.85</v>
       </c>
-      <c r="G63" s="2">
+      <c r="G63">
         <v>22.6</v>
       </c>
-      <c r="H63" s="2">
+      <c r="H63">
         <v>18.5</v>
       </c>
-      <c r="J63" s="2">
+      <c r="J63" s="4">
         <v>43972</v>
       </c>
-      <c r="K63" s="2">
+      <c r="K63" s="4">
         <v>44014</v>
       </c>
       <c r="L63">
@@ -3046,27 +3483,27 @@
         <v>3</v>
       </c>
       <c r="C64" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D64">
         <v>14</v>
       </c>
-      <c r="E64" s="2">
+      <c r="E64">
         <v>1.46</v>
       </c>
-      <c r="F64" s="2">
+      <c r="F64">
         <v>1.05</v>
       </c>
-      <c r="G64" s="2">
+      <c r="G64">
         <v>14.6</v>
       </c>
-      <c r="H64" s="2">
+      <c r="H64">
         <v>10.5</v>
       </c>
-      <c r="J64" s="2">
+      <c r="J64" s="4">
         <v>44370</v>
       </c>
-      <c r="K64" s="2">
+      <c r="K64" s="4">
         <v>44426</v>
       </c>
       <c r="L64">
@@ -3093,27 +3530,27 @@
         <v>4</v>
       </c>
       <c r="C65" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D65">
         <v>16</v>
       </c>
-      <c r="E65" s="2">
+      <c r="E65">
         <v>2.59</v>
       </c>
-      <c r="F65" s="2">
+      <c r="F65">
         <v>2.34</v>
       </c>
-      <c r="G65" s="2">
+      <c r="G65">
         <v>25.9</v>
       </c>
-      <c r="H65" s="2">
+      <c r="H65">
         <v>23.4</v>
       </c>
-      <c r="J65" s="2">
+      <c r="J65" s="4">
         <v>44252</v>
       </c>
-      <c r="K65" s="2">
+      <c r="K65" s="4">
         <v>44322</v>
       </c>
       <c r="L65">
@@ -3137,27 +3574,27 @@
         <v>2</v>
       </c>
       <c r="C66" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D66">
         <v>14</v>
       </c>
-      <c r="E66" s="2">
+      <c r="E66">
         <v>3.55</v>
       </c>
-      <c r="F66" s="2">
+      <c r="F66">
         <v>2.76</v>
       </c>
-      <c r="G66" s="2">
+      <c r="G66">
         <v>35.5</v>
       </c>
-      <c r="H66" s="2">
+      <c r="H66">
         <v>27.6</v>
       </c>
-      <c r="J66" s="2">
+      <c r="J66" s="4">
         <v>43875</v>
       </c>
-      <c r="K66" s="2">
+      <c r="K66" s="4">
         <v>43924</v>
       </c>
       <c r="L66">
@@ -3184,27 +3621,27 @@
         <v>4</v>
       </c>
       <c r="C67" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D67">
         <v>15</v>
       </c>
-      <c r="E67" s="2">
+      <c r="E67">
         <v>1.99</v>
       </c>
-      <c r="F67" s="2">
+      <c r="F67">
         <v>1.66</v>
       </c>
-      <c r="G67" s="2">
+      <c r="G67">
         <v>19.899999999999999</v>
       </c>
-      <c r="H67" s="2">
+      <c r="H67">
         <v>16.600000000000001</v>
       </c>
-      <c r="J67" s="2">
+      <c r="J67" s="4">
         <v>44083</v>
       </c>
-      <c r="K67" s="2">
+      <c r="K67" s="4">
         <v>44132</v>
       </c>
       <c r="L67">
@@ -3228,27 +3665,27 @@
         <v>5</v>
       </c>
       <c r="C68" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D68">
         <v>13</v>
       </c>
-      <c r="E68" s="2">
+      <c r="E68">
         <v>3.19</v>
       </c>
-      <c r="F68" s="2">
+      <c r="F68">
         <v>2.4300000000000002</v>
       </c>
-      <c r="G68" s="2">
+      <c r="G68">
         <v>31.9</v>
       </c>
-      <c r="H68" s="2">
+      <c r="H68">
         <v>24.3</v>
       </c>
-      <c r="J68" s="2">
+      <c r="J68" s="4">
         <v>43854</v>
       </c>
-      <c r="K68" s="2">
+      <c r="K68" s="4">
         <v>43896</v>
       </c>
       <c r="L68">
@@ -3272,27 +3709,27 @@
         <v>2</v>
       </c>
       <c r="C69" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D69">
         <v>13</v>
       </c>
-      <c r="E69" s="2">
+      <c r="E69">
         <v>0.78</v>
       </c>
-      <c r="F69" s="2">
+      <c r="F69">
         <v>0.56000000000000005</v>
       </c>
-      <c r="G69" s="2">
+      <c r="G69">
         <v>7.8</v>
       </c>
-      <c r="H69" s="2">
+      <c r="H69">
         <v>5.6</v>
       </c>
-      <c r="J69" s="2">
+      <c r="J69" s="4">
         <v>44166</v>
       </c>
-      <c r="K69" s="2">
+      <c r="K69" s="4">
         <v>44180</v>
       </c>
       <c r="L69">
@@ -3319,27 +3756,27 @@
         <v>3</v>
       </c>
       <c r="C70" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D70">
         <v>17</v>
       </c>
-      <c r="E70" s="2">
+      <c r="E70">
         <v>2.9</v>
       </c>
-      <c r="F70" s="2">
+      <c r="F70">
         <v>2.2799999999999998</v>
       </c>
-      <c r="G70" s="2">
+      <c r="G70">
         <v>29</v>
       </c>
-      <c r="H70" s="2">
+      <c r="H70">
         <v>22.8</v>
       </c>
-      <c r="J70" s="2">
+      <c r="J70" s="4">
         <v>44370</v>
       </c>
-      <c r="K70" s="2">
+      <c r="K70" s="4">
         <v>44398</v>
       </c>
       <c r="L70">
@@ -3363,27 +3800,27 @@
         <v>2</v>
       </c>
       <c r="C71" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D71">
         <v>14</v>
       </c>
-      <c r="E71" s="2">
+      <c r="E71">
         <v>2.72</v>
       </c>
-      <c r="F71" s="2">
+      <c r="F71">
         <v>2.17</v>
       </c>
-      <c r="G71" s="2">
+      <c r="G71">
         <v>27.2</v>
       </c>
-      <c r="H71" s="2">
+      <c r="H71">
         <v>21.7</v>
       </c>
-      <c r="J71" s="2">
+      <c r="J71" s="4">
         <v>44412</v>
       </c>
-      <c r="K71" s="2">
+      <c r="K71" s="4">
         <v>44545</v>
       </c>
       <c r="L71">
@@ -3407,27 +3844,27 @@
         <v>4</v>
       </c>
       <c r="C72" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D72">
         <v>18</v>
       </c>
-      <c r="E72" s="2">
+      <c r="E72">
         <v>1.08</v>
       </c>
-      <c r="F72" s="2">
+      <c r="F72">
         <v>0.81</v>
       </c>
-      <c r="G72" s="2">
+      <c r="G72">
         <v>10.8</v>
       </c>
-      <c r="H72" s="2">
+      <c r="H72">
         <v>8.1</v>
       </c>
-      <c r="J72" s="2">
+      <c r="J72" s="4">
         <v>44007</v>
       </c>
-      <c r="K72" s="2">
+      <c r="K72" s="4">
         <v>44021</v>
       </c>
       <c r="L72">
@@ -3454,27 +3891,27 @@
         <v>3</v>
       </c>
       <c r="C73" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="D73">
         <v>15</v>
       </c>
-      <c r="E73" s="2">
+      <c r="E73">
         <v>1.95</v>
       </c>
-      <c r="F73" s="2">
+      <c r="F73">
         <v>1.41</v>
       </c>
-      <c r="G73" s="2">
+      <c r="G73">
         <v>19.5</v>
       </c>
-      <c r="H73" s="2">
+      <c r="H73">
         <v>14.1</v>
       </c>
-      <c r="J73" s="2">
+      <c r="J73" s="4">
         <v>44287</v>
       </c>
-      <c r="K73" s="2">
+      <c r="K73" s="4">
         <v>44315</v>
       </c>
       <c r="L73">
@@ -3498,27 +3935,27 @@
         <v>4</v>
       </c>
       <c r="C74" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D74">
         <v>16</v>
       </c>
-      <c r="E74" s="2">
+      <c r="E74">
         <v>2.25</v>
       </c>
-      <c r="F74" s="2">
+      <c r="F74">
         <v>1.91</v>
       </c>
-      <c r="G74" s="2">
+      <c r="G74">
         <v>22.5</v>
       </c>
-      <c r="H74" s="2">
+      <c r="H74">
         <v>19.100000000000001</v>
       </c>
-      <c r="J74" s="2">
+      <c r="J74" s="4">
         <v>44321</v>
       </c>
-      <c r="K74" s="2">
+      <c r="K74" s="4">
         <v>44342</v>
       </c>
       <c r="L74">
@@ -3542,27 +3979,27 @@
         <v>4</v>
       </c>
       <c r="C75" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D75">
         <v>15</v>
       </c>
-      <c r="E75" s="2">
+      <c r="E75">
         <v>1.01</v>
       </c>
-      <c r="F75" s="2">
+      <c r="F75">
         <v>0.91</v>
       </c>
-      <c r="G75" s="2">
+      <c r="G75">
         <v>10.1</v>
       </c>
-      <c r="H75" s="2">
+      <c r="H75">
         <v>9.1</v>
       </c>
-      <c r="J75" s="2">
+      <c r="J75" s="4">
         <v>44056</v>
       </c>
-      <c r="K75" s="2">
+      <c r="K75" s="4">
         <v>44161</v>
       </c>
       <c r="L75">
@@ -3586,27 +4023,27 @@
         <v>3</v>
       </c>
       <c r="C76" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D76">
         <v>16</v>
       </c>
-      <c r="E76" s="2">
+      <c r="E76">
         <v>2.67</v>
       </c>
-      <c r="F76" s="2">
+      <c r="F76">
         <v>2.15</v>
       </c>
-      <c r="G76" s="2">
+      <c r="G76">
         <v>26.7</v>
       </c>
-      <c r="H76" s="2">
+      <c r="H76">
         <v>21.5</v>
       </c>
-      <c r="J76" s="2">
+      <c r="J76" s="4">
         <v>44134</v>
       </c>
-      <c r="K76" s="2">
+      <c r="K76" s="4">
         <v>44176</v>
       </c>
       <c r="L76">
@@ -3630,27 +4067,27 @@
         <v>4</v>
       </c>
       <c r="C77" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D77">
         <v>15</v>
       </c>
-      <c r="E77" s="2">
+      <c r="E77">
         <v>2.91</v>
       </c>
-      <c r="F77" s="2">
+      <c r="F77">
         <v>2.2400000000000002</v>
       </c>
-      <c r="G77" s="2">
+      <c r="G77">
         <v>29.1</v>
       </c>
-      <c r="H77" s="2">
+      <c r="H77">
         <v>22.4</v>
       </c>
-      <c r="J77" s="2">
+      <c r="J77" s="4">
         <v>43949</v>
       </c>
-      <c r="K77" s="2">
+      <c r="K77" s="4">
         <v>43977</v>
       </c>
       <c r="L77">
@@ -3674,27 +4111,27 @@
         <v>4</v>
       </c>
       <c r="C78" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D78">
         <v>16</v>
       </c>
-      <c r="E78" s="2">
+      <c r="E78">
         <v>3.14</v>
       </c>
-      <c r="F78" s="2">
+      <c r="F78">
         <v>2.6</v>
       </c>
-      <c r="G78" s="2">
+      <c r="G78">
         <v>31.4</v>
       </c>
-      <c r="H78" s="2">
+      <c r="H78">
         <v>26</v>
       </c>
-      <c r="J78" s="2">
+      <c r="J78" s="4">
         <v>44180</v>
       </c>
-      <c r="K78" s="2">
+      <c r="K78" s="4">
         <v>44215</v>
       </c>
       <c r="L78">
@@ -3718,27 +4155,27 @@
         <v>2</v>
       </c>
       <c r="C79" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D79">
         <v>13</v>
       </c>
-      <c r="E79" s="2">
+      <c r="E79">
         <v>2.93</v>
       </c>
-      <c r="F79" s="2">
+      <c r="F79">
         <v>2.39</v>
       </c>
-      <c r="G79" s="2">
+      <c r="G79">
         <v>29.3</v>
       </c>
-      <c r="H79" s="2">
+      <c r="H79">
         <v>23.9</v>
       </c>
-      <c r="J79" s="2">
+      <c r="J79" s="4">
         <v>43984</v>
       </c>
-      <c r="K79" s="2">
+      <c r="K79" s="4">
         <v>44089</v>
       </c>
       <c r="L79">
@@ -3762,27 +4199,27 @@
         <v>2</v>
       </c>
       <c r="C80" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D80">
         <v>15</v>
       </c>
-      <c r="E80" s="2">
+      <c r="E80">
         <v>3.79</v>
       </c>
-      <c r="F80" s="2">
+      <c r="F80">
         <v>3.01</v>
       </c>
-      <c r="G80" s="2">
+      <c r="G80">
         <v>37.9</v>
       </c>
-      <c r="H80" s="2">
+      <c r="H80">
         <v>30.1</v>
       </c>
-      <c r="J80" s="2">
+      <c r="J80" s="4">
         <v>43943</v>
       </c>
-      <c r="K80" s="2">
+      <c r="K80" s="4">
         <v>43999</v>
       </c>
       <c r="L80">
@@ -3806,27 +4243,27 @@
         <v>5</v>
       </c>
       <c r="C81" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D81">
         <v>17</v>
       </c>
-      <c r="E81" s="2">
+      <c r="E81">
         <v>2.42</v>
       </c>
-      <c r="F81" s="2">
+      <c r="F81">
         <v>1.87</v>
       </c>
-      <c r="G81" s="2">
+      <c r="G81">
         <v>24.2</v>
       </c>
-      <c r="H81" s="2">
+      <c r="H81">
         <v>18.7</v>
       </c>
-      <c r="J81" s="2">
+      <c r="J81" s="4">
         <v>44084</v>
       </c>
-      <c r="K81" s="2">
+      <c r="K81" s="4">
         <v>44119</v>
       </c>
       <c r="L81">
@@ -3850,27 +4287,27 @@
         <v>2</v>
       </c>
       <c r="C82" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D82">
         <v>13</v>
       </c>
-      <c r="E82" s="2">
+      <c r="E82">
         <v>2.65</v>
       </c>
-      <c r="F82" s="2">
+      <c r="F82">
         <v>2.23</v>
       </c>
-      <c r="G82" s="2">
+      <c r="G82">
         <v>26.5</v>
       </c>
-      <c r="H82" s="2">
+      <c r="H82">
         <v>22.3</v>
       </c>
-      <c r="J82" s="2">
+      <c r="J82" s="4">
         <v>44028</v>
       </c>
-      <c r="K82" s="2">
+      <c r="K82" s="4">
         <v>44077</v>
       </c>
       <c r="L82">
@@ -3894,27 +4331,27 @@
         <v>5</v>
       </c>
       <c r="C83" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D83">
         <v>16</v>
       </c>
-      <c r="E83" s="2">
+      <c r="E83">
         <v>1.98</v>
       </c>
-      <c r="F83" s="2">
+      <c r="F83">
         <v>1.77</v>
       </c>
-      <c r="G83" s="2">
+      <c r="G83">
         <v>19.8</v>
       </c>
-      <c r="H83" s="2">
+      <c r="H83">
         <v>17.7</v>
       </c>
-      <c r="J83" s="2">
+      <c r="J83" s="4">
         <v>44463</v>
       </c>
-      <c r="K83" s="2">
+      <c r="K83" s="4">
         <v>44505</v>
       </c>
       <c r="L83">
@@ -3938,27 +4375,27 @@
         <v>3</v>
       </c>
       <c r="C84" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D84">
         <v>17</v>
       </c>
-      <c r="E84" s="2">
+      <c r="E84">
         <v>3.11</v>
       </c>
-      <c r="F84" s="2">
+      <c r="F84">
         <v>2.4</v>
       </c>
-      <c r="G84" s="2">
+      <c r="G84">
         <v>31.1</v>
       </c>
-      <c r="H84" s="2">
+      <c r="H84">
         <v>24</v>
       </c>
-      <c r="J84" s="2">
+      <c r="J84" s="4">
         <v>44435</v>
       </c>
-      <c r="K84" s="2">
+      <c r="K84" s="4">
         <v>44463</v>
       </c>
       <c r="L84">
@@ -3985,27 +4422,27 @@
         <v>5</v>
       </c>
       <c r="C85" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D85">
         <v>16</v>
       </c>
-      <c r="E85" s="2">
+      <c r="E85">
         <v>3.05</v>
       </c>
-      <c r="F85" s="2">
+      <c r="F85">
         <v>2.2999999999999998</v>
       </c>
-      <c r="G85" s="2">
+      <c r="G85">
         <v>30.5</v>
       </c>
-      <c r="H85" s="2">
+      <c r="H85">
         <v>23</v>
       </c>
-      <c r="J85" s="2">
+      <c r="J85" s="4">
         <v>44252</v>
       </c>
-      <c r="K85" s="2">
+      <c r="K85" s="4">
         <v>44301</v>
       </c>
       <c r="L85">
@@ -4029,27 +4466,27 @@
         <v>2</v>
       </c>
       <c r="C86" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D86">
         <v>17</v>
       </c>
-      <c r="E86" s="2">
+      <c r="E86">
         <v>2.36</v>
       </c>
-      <c r="F86" s="2">
+      <c r="F86">
         <v>1.99</v>
       </c>
-      <c r="G86" s="2">
+      <c r="G86">
         <v>23.6</v>
       </c>
-      <c r="H86" s="2">
+      <c r="H86">
         <v>19.899999999999999</v>
       </c>
-      <c r="J86" s="2">
+      <c r="J86" s="4">
         <v>44287</v>
       </c>
-      <c r="K86" s="2">
+      <c r="K86" s="4">
         <v>44329</v>
       </c>
       <c r="L86">
@@ -4076,27 +4513,27 @@
         <v>2</v>
       </c>
       <c r="C87" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D87">
         <v>15</v>
       </c>
-      <c r="E87" s="2">
+      <c r="E87">
         <v>1.08</v>
       </c>
-      <c r="F87" s="2">
+      <c r="F87">
         <v>0.59</v>
       </c>
-      <c r="G87" s="2">
+      <c r="G87">
         <v>10.8</v>
       </c>
-      <c r="H87" s="2">
+      <c r="H87">
         <v>5.9</v>
       </c>
-      <c r="J87" s="2">
+      <c r="J87" s="4">
         <v>44007</v>
       </c>
-      <c r="K87" s="2">
+      <c r="K87" s="4">
         <v>44056</v>
       </c>
       <c r="L87">
@@ -4123,27 +4560,27 @@
         <v>3</v>
       </c>
       <c r="C88" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D88">
         <v>18</v>
       </c>
-      <c r="E88" s="2">
+      <c r="E88">
         <v>2.23</v>
       </c>
-      <c r="F88" s="2">
+      <c r="F88">
         <v>1.72</v>
       </c>
-      <c r="G88" s="2">
+      <c r="G88">
         <v>22.3</v>
       </c>
-      <c r="H88" s="2">
+      <c r="H88">
         <v>17.2</v>
       </c>
-      <c r="J88" s="2">
+      <c r="J88" s="4">
         <v>44378</v>
       </c>
-      <c r="K88" s="2">
+      <c r="K88" s="4">
         <v>44399</v>
       </c>
       <c r="L88">
@@ -4170,27 +4607,27 @@
         <v>5</v>
       </c>
       <c r="C89" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D89">
         <v>11</v>
       </c>
-      <c r="E89" s="2">
+      <c r="E89">
         <v>1.25</v>
       </c>
-      <c r="F89" s="2">
+      <c r="F89">
         <v>1.04</v>
       </c>
-      <c r="G89" s="2">
+      <c r="G89">
         <v>12.5</v>
       </c>
-      <c r="H89" s="2">
+      <c r="H89">
         <v>10.4</v>
       </c>
-      <c r="J89" s="2">
+      <c r="J89" s="4">
         <v>44145</v>
       </c>
-      <c r="K89" s="2">
+      <c r="K89" s="4">
         <v>44180</v>
       </c>
       <c r="L89">
@@ -4219,22 +4656,22 @@
       <c r="D90">
         <v>14</v>
       </c>
-      <c r="E90" s="2">
+      <c r="E90">
         <v>2.88</v>
       </c>
-      <c r="F90" s="2">
+      <c r="F90">
         <v>2.5</v>
       </c>
-      <c r="G90" s="2">
+      <c r="G90">
         <v>28.8</v>
       </c>
-      <c r="H90" s="2">
+      <c r="H90">
         <v>25</v>
       </c>
-      <c r="J90" s="2">
+      <c r="J90" s="4">
         <v>44400</v>
       </c>
-      <c r="K90" s="2">
+      <c r="K90" s="4">
         <v>44442</v>
       </c>
       <c r="L90">
@@ -4261,27 +4698,27 @@
         <v>4</v>
       </c>
       <c r="C91" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D91">
         <v>13</v>
       </c>
-      <c r="E91" s="2">
+      <c r="E91">
         <v>2.96</v>
       </c>
-      <c r="F91" s="2">
+      <c r="F91">
         <v>2.17</v>
       </c>
-      <c r="G91" s="2">
+      <c r="G91">
         <v>29.6</v>
       </c>
-      <c r="H91" s="2">
+      <c r="H91">
         <v>21.7</v>
       </c>
-      <c r="J91" s="2">
+      <c r="J91" s="4">
         <v>44342</v>
       </c>
-      <c r="K91" s="2">
+      <c r="K91" s="4">
         <v>44370</v>
       </c>
       <c r="L91">
@@ -4308,27 +4745,27 @@
         <v>3</v>
       </c>
       <c r="C92" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D92">
         <v>15</v>
       </c>
-      <c r="E92" s="2">
+      <c r="E92">
         <v>1.54</v>
       </c>
-      <c r="F92" s="2">
+      <c r="F92">
         <v>1.23</v>
       </c>
-      <c r="G92" s="2">
+      <c r="G92">
         <v>15.4</v>
       </c>
-      <c r="H92" s="2">
+      <c r="H92">
         <v>12.3</v>
       </c>
-      <c r="J92" s="2">
+      <c r="J92" s="4">
         <v>43889</v>
       </c>
-      <c r="K92" s="2">
+      <c r="K92" s="4">
         <v>43945</v>
       </c>
       <c r="L92">
@@ -4352,27 +4789,27 @@
         <v>3</v>
       </c>
       <c r="C93" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D93">
         <v>16</v>
       </c>
-      <c r="E93" s="2">
+      <c r="E93">
         <v>1.32</v>
       </c>
-      <c r="F93" s="2">
+      <c r="F93">
         <v>0.87</v>
       </c>
-      <c r="G93" s="2">
+      <c r="G93">
         <v>13.2</v>
       </c>
-      <c r="H93" s="2">
+      <c r="H93">
         <v>8.6999999999999993</v>
       </c>
-      <c r="J93" s="2">
+      <c r="J93" s="4">
         <v>44470</v>
       </c>
-      <c r="K93" s="2">
+      <c r="K93" s="4">
         <v>44505</v>
       </c>
       <c r="L93">
@@ -4396,27 +4833,27 @@
         <v>3</v>
       </c>
       <c r="C94" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D94">
         <v>13</v>
       </c>
-      <c r="E94" s="2">
+      <c r="E94">
         <v>3.13</v>
       </c>
-      <c r="F94" s="2">
+      <c r="F94">
         <v>2.68</v>
       </c>
-      <c r="G94" s="2">
+      <c r="G94">
         <v>31.3</v>
       </c>
-      <c r="H94" s="2">
+      <c r="H94">
         <v>26.8</v>
       </c>
-      <c r="J94" s="2">
+      <c r="J94" s="4">
         <v>44173</v>
       </c>
-      <c r="K94" s="2">
+      <c r="K94" s="4">
         <v>44222</v>
       </c>
       <c r="L94">
@@ -4443,27 +4880,27 @@
         <v>2</v>
       </c>
       <c r="C95" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D95">
         <v>12</v>
       </c>
-      <c r="E95" s="2">
+      <c r="E95">
         <v>3.32</v>
       </c>
-      <c r="F95" s="2">
+      <c r="F95">
         <v>2.46</v>
       </c>
-      <c r="G95" s="2">
+      <c r="G95">
         <v>33.200000000000003</v>
       </c>
-      <c r="H95" s="2">
+      <c r="H95">
         <v>24.6</v>
       </c>
-      <c r="J95" s="2">
+      <c r="J95" s="4">
         <v>44069</v>
       </c>
-      <c r="K95" s="2">
+      <c r="K95" s="4">
         <v>44251</v>
       </c>
       <c r="L95">
@@ -4487,27 +4924,27 @@
         <v>2</v>
       </c>
       <c r="C96" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D96">
         <v>12</v>
       </c>
-      <c r="E96" s="2">
+      <c r="E96">
         <v>3.74</v>
       </c>
-      <c r="F96" s="2">
+      <c r="F96">
         <v>2.99</v>
       </c>
-      <c r="G96" s="2">
+      <c r="G96">
         <v>37.4</v>
       </c>
-      <c r="H96" s="2">
+      <c r="H96">
         <v>29.9</v>
       </c>
-      <c r="J96" s="2">
+      <c r="J96" s="4">
         <v>44243</v>
       </c>
-      <c r="K96" s="2">
+      <c r="K96" s="4">
         <v>44285</v>
       </c>
       <c r="L96">
@@ -4536,22 +4973,22 @@
       <c r="D97">
         <v>12</v>
       </c>
-      <c r="E97" s="2">
+      <c r="E97">
         <v>1.94</v>
       </c>
-      <c r="F97" s="2">
+      <c r="F97">
         <v>1.59</v>
       </c>
-      <c r="G97" s="2">
+      <c r="G97">
         <v>19.399999999999999</v>
       </c>
-      <c r="H97" s="2">
+      <c r="H97">
         <v>15.9</v>
       </c>
-      <c r="J97" s="2">
+      <c r="J97" s="4">
         <v>44139</v>
       </c>
-      <c r="K97" s="2">
+      <c r="K97" s="4">
         <v>44167</v>
       </c>
       <c r="L97">
@@ -4578,27 +5015,27 @@
         <v>5</v>
       </c>
       <c r="C98" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D98">
         <v>12</v>
       </c>
-      <c r="E98" s="2">
+      <c r="E98">
         <v>0.75</v>
       </c>
-      <c r="F98" s="2">
+      <c r="F98">
         <v>0.65</v>
       </c>
-      <c r="G98" s="2">
+      <c r="G98">
         <v>7.5</v>
       </c>
-      <c r="H98" s="2">
+      <c r="H98">
         <v>6.5</v>
       </c>
-      <c r="J98" s="2">
+      <c r="J98" s="4">
         <v>44281</v>
       </c>
-      <c r="K98" s="2">
+      <c r="K98" s="4">
         <v>44344</v>
       </c>
       <c r="L98">
@@ -4625,27 +5062,27 @@
         <v>4</v>
       </c>
       <c r="C99" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D99">
         <v>15</v>
       </c>
-      <c r="E99" s="2">
+      <c r="E99">
         <v>2.36</v>
       </c>
-      <c r="F99" s="2">
+      <c r="F99">
         <v>1.95</v>
       </c>
-      <c r="G99" s="2">
+      <c r="G99">
         <v>23.6</v>
       </c>
-      <c r="H99" s="2">
+      <c r="H99">
         <v>19.5</v>
       </c>
-      <c r="J99" s="2">
+      <c r="J99" s="4">
         <v>43909</v>
       </c>
-      <c r="K99" s="2">
+      <c r="K99" s="4">
         <v>43979</v>
       </c>
       <c r="L99">
@@ -4672,27 +5109,27 @@
         <v>4</v>
       </c>
       <c r="C100" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D100">
         <v>14</v>
       </c>
-      <c r="E100" s="2">
+      <c r="E100">
         <v>0.85</v>
       </c>
-      <c r="F100" s="2">
+      <c r="F100">
         <v>0.94</v>
       </c>
-      <c r="G100" s="2">
+      <c r="G100">
         <v>8.5</v>
       </c>
-      <c r="H100" s="2">
+      <c r="H100">
         <v>9.4</v>
       </c>
-      <c r="J100" s="2">
+      <c r="J100" s="4">
         <v>44005</v>
       </c>
-      <c r="K100" s="2">
+      <c r="K100" s="4">
         <v>44089</v>
       </c>
       <c r="L100">
@@ -4719,27 +5156,27 @@
         <v>3</v>
       </c>
       <c r="C101" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D101">
         <v>11</v>
       </c>
-      <c r="E101" s="2">
+      <c r="E101">
         <v>1.46</v>
       </c>
-      <c r="F101" s="2">
+      <c r="F101">
         <v>1.31</v>
       </c>
-      <c r="G101" s="2">
+      <c r="G101">
         <v>14.6</v>
       </c>
-      <c r="H101" s="2">
+      <c r="H101">
         <v>13.1</v>
       </c>
-      <c r="J101" s="2">
+      <c r="J101" s="4">
         <v>44273</v>
       </c>
-      <c r="K101" s="2">
+      <c r="K101" s="4">
         <v>44315</v>
       </c>
       <c r="L101">
@@ -4766,27 +5203,27 @@
         <v>5</v>
       </c>
       <c r="C102" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D102">
         <v>16</v>
       </c>
-      <c r="E102" s="2">
+      <c r="E102">
         <v>2.21</v>
       </c>
-      <c r="F102" s="2">
+      <c r="F102">
         <v>1.77</v>
       </c>
-      <c r="G102" s="2">
+      <c r="G102">
         <v>22.1</v>
       </c>
-      <c r="H102" s="2">
+      <c r="H102">
         <v>17.7</v>
       </c>
-      <c r="J102" s="2">
+      <c r="J102" s="4">
         <v>43867</v>
       </c>
-      <c r="K102" s="2">
+      <c r="K102" s="4">
         <v>43895</v>
       </c>
       <c r="L102">
@@ -4813,27 +5250,27 @@
         <v>4</v>
       </c>
       <c r="C103" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D103">
         <v>13</v>
       </c>
-      <c r="E103" s="2">
+      <c r="E103">
         <v>1.06</v>
       </c>
-      <c r="F103" s="2">
+      <c r="F103">
         <v>0.88</v>
       </c>
-      <c r="G103" s="2">
+      <c r="G103">
         <v>10.6</v>
       </c>
-      <c r="H103" s="2">
+      <c r="H103">
         <v>8.8000000000000007</v>
       </c>
-      <c r="J103" s="2">
+      <c r="J103" s="4">
         <v>44315</v>
       </c>
-      <c r="K103" s="2">
+      <c r="K103" s="4">
         <v>44350</v>
       </c>
       <c r="L103">
@@ -4857,27 +5294,27 @@
         <v>5</v>
       </c>
       <c r="C104" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D104">
         <v>15</v>
       </c>
-      <c r="E104" s="2">
+      <c r="E104">
         <v>2.02</v>
       </c>
-      <c r="F104" s="2">
+      <c r="F104">
         <v>1.52</v>
       </c>
-      <c r="G104" s="2">
+      <c r="G104">
         <v>20.2</v>
       </c>
-      <c r="H104" s="2">
+      <c r="H104">
         <v>15.2</v>
       </c>
-      <c r="J104" s="2">
+      <c r="J104" s="4">
         <v>44124</v>
       </c>
-      <c r="K104" s="2">
+      <c r="K104" s="4">
         <v>44173</v>
       </c>
       <c r="L104">
@@ -4904,27 +5341,27 @@
         <v>3</v>
       </c>
       <c r="C105" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D105">
         <v>16</v>
       </c>
-      <c r="E105" s="2">
+      <c r="E105">
         <v>1.19</v>
       </c>
-      <c r="F105" s="2">
+      <c r="F105">
         <v>0.95</v>
       </c>
-      <c r="G105" s="2">
+      <c r="G105">
         <v>11.9</v>
       </c>
-      <c r="H105" s="2">
+      <c r="H105">
         <v>9.5</v>
       </c>
-      <c r="J105" s="2">
+      <c r="J105" s="4">
         <v>44007</v>
       </c>
-      <c r="K105" s="2">
+      <c r="K105" s="4">
         <v>44028</v>
       </c>
       <c r="L105">
@@ -4951,27 +5388,27 @@
         <v>4</v>
       </c>
       <c r="C106" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D106">
         <v>15</v>
       </c>
-      <c r="E106" s="2">
+      <c r="E106">
         <v>1.0900000000000001</v>
       </c>
-      <c r="F106" s="2">
+      <c r="F106">
         <v>0.84</v>
       </c>
-      <c r="G106" s="2">
+      <c r="G106">
         <v>10.9</v>
       </c>
-      <c r="H106" s="2">
+      <c r="H106">
         <v>8.4</v>
       </c>
-      <c r="J106" s="2">
+      <c r="J106" s="4">
         <v>44260</v>
       </c>
-      <c r="K106" s="2">
+      <c r="K106" s="4">
         <v>44428</v>
       </c>
       <c r="L106">
@@ -4995,27 +5432,27 @@
         <v>2</v>
       </c>
       <c r="C107" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D107">
         <v>17</v>
       </c>
-      <c r="E107" s="2">
+      <c r="E107">
         <v>1.35</v>
       </c>
-      <c r="F107" s="2">
+      <c r="F107">
         <v>0.96</v>
       </c>
-      <c r="G107" s="2">
+      <c r="G107">
         <v>13.5</v>
       </c>
-      <c r="H107" s="2">
+      <c r="H107">
         <v>9.6</v>
       </c>
-      <c r="J107" s="2">
+      <c r="J107" s="4">
         <v>44427</v>
       </c>
-      <c r="K107" s="2">
+      <c r="K107" s="4">
         <v>44483</v>
       </c>
       <c r="L107">
@@ -5039,27 +5476,27 @@
         <v>5</v>
       </c>
       <c r="C108" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D108">
         <v>12</v>
       </c>
-      <c r="E108" s="2">
+      <c r="E108">
         <v>3.19</v>
       </c>
-      <c r="F108" s="2">
+      <c r="F108">
         <v>2.5299999999999998</v>
       </c>
-      <c r="G108" s="2">
+      <c r="G108">
         <v>31.9</v>
       </c>
-      <c r="H108" s="2">
+      <c r="H108">
         <v>25.3</v>
       </c>
-      <c r="J108" s="2">
+      <c r="J108" s="4">
         <v>43991</v>
       </c>
-      <c r="K108" s="2">
+      <c r="K108" s="4">
         <v>44040</v>
       </c>
       <c r="L108">
@@ -5083,27 +5520,27 @@
         <v>3</v>
       </c>
       <c r="C109" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D109">
         <v>15</v>
       </c>
-      <c r="E109" s="2">
+      <c r="E109">
         <v>1.71</v>
       </c>
-      <c r="F109" s="2">
+      <c r="F109">
         <v>1.26</v>
       </c>
-      <c r="G109" s="2">
+      <c r="G109">
         <v>17.100000000000001</v>
       </c>
-      <c r="H109" s="2">
+      <c r="H109">
         <v>12.6</v>
       </c>
-      <c r="J109" s="2">
+      <c r="J109" s="4">
         <v>44418</v>
       </c>
-      <c r="K109" s="2">
+      <c r="K109" s="4">
         <v>44439</v>
       </c>
       <c r="L109">
@@ -5127,27 +5564,27 @@
         <v>2</v>
       </c>
       <c r="C110" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D110">
         <v>14</v>
       </c>
-      <c r="E110" s="2">
+      <c r="E110">
         <v>2.69</v>
       </c>
-      <c r="F110" s="2">
+      <c r="F110">
         <v>2.17</v>
       </c>
-      <c r="G110" s="2">
+      <c r="G110">
         <v>26.9</v>
       </c>
-      <c r="H110" s="2">
+      <c r="H110">
         <v>21.7</v>
       </c>
-      <c r="J110" s="2">
+      <c r="J110" s="4">
         <v>44307</v>
       </c>
-      <c r="K110" s="2">
+      <c r="K110" s="4">
         <v>44377</v>
       </c>
       <c r="L110">
@@ -5171,27 +5608,27 @@
         <v>4</v>
       </c>
       <c r="C111" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D111">
         <v>15</v>
       </c>
-      <c r="E111" s="2">
+      <c r="E111">
         <v>3.04</v>
       </c>
-      <c r="F111" s="2">
+      <c r="F111">
         <v>2.5099999999999998</v>
       </c>
-      <c r="G111" s="2">
+      <c r="G111">
         <v>30.4</v>
       </c>
-      <c r="H111" s="2">
+      <c r="H111">
         <v>25.1</v>
       </c>
-      <c r="J111" s="2">
+      <c r="J111" s="4">
         <v>44421</v>
       </c>
-      <c r="K111" s="2">
+      <c r="K111" s="4">
         <v>44491</v>
       </c>
       <c r="L111">
@@ -5215,27 +5652,27 @@
         <v>5</v>
       </c>
       <c r="C112" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D112">
         <v>13</v>
       </c>
-      <c r="E112" s="2">
+      <c r="E112">
         <v>1.84</v>
       </c>
-      <c r="F112" s="2">
+      <c r="F112">
         <v>1.64</v>
       </c>
-      <c r="G112" s="2">
+      <c r="G112">
         <v>18.399999999999999</v>
       </c>
-      <c r="H112" s="2">
+      <c r="H112">
         <v>16.399999999999999</v>
       </c>
-      <c r="J112" s="2">
+      <c r="J112" s="4">
         <v>44327</v>
       </c>
-      <c r="K112" s="2">
+      <c r="K112" s="4">
         <v>44404</v>
       </c>
       <c r="L112">
@@ -5259,27 +5696,27 @@
         <v>5</v>
       </c>
       <c r="C113" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D113">
         <v>13</v>
       </c>
-      <c r="E113" s="2">
+      <c r="E113">
         <v>1.35</v>
       </c>
-      <c r="F113" s="2">
+      <c r="F113">
         <v>0.96</v>
       </c>
-      <c r="G113" s="2">
+      <c r="G113">
         <v>13.5</v>
       </c>
-      <c r="H113" s="2">
+      <c r="H113">
         <v>9.6</v>
       </c>
-      <c r="J113" s="2">
+      <c r="J113" s="4">
         <v>44019</v>
       </c>
-      <c r="K113" s="2">
+      <c r="K113" s="4">
         <v>44138</v>
       </c>
       <c r="L113">
@@ -5303,27 +5740,27 @@
         <v>2</v>
       </c>
       <c r="C114" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="D114">
         <v>13</v>
       </c>
-      <c r="E114" s="2">
+      <c r="E114">
         <v>1.45</v>
       </c>
-      <c r="F114" s="2">
+      <c r="F114">
         <v>1.32</v>
       </c>
-      <c r="G114" s="2">
+      <c r="G114">
         <v>14.5</v>
       </c>
-      <c r="H114" s="2">
+      <c r="H114">
         <v>13.2</v>
       </c>
-      <c r="J114" s="2">
+      <c r="J114" s="4">
         <v>44092</v>
       </c>
-      <c r="K114" s="2">
+      <c r="K114" s="4">
         <v>44120</v>
       </c>
       <c r="L114">
@@ -5347,27 +5784,27 @@
         <v>5</v>
       </c>
       <c r="C115" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D115">
         <v>17</v>
       </c>
-      <c r="E115" s="2">
+      <c r="E115">
         <v>2.2000000000000002</v>
       </c>
-      <c r="F115" s="2">
+      <c r="F115">
         <v>1.93</v>
       </c>
-      <c r="G115" s="2">
+      <c r="G115">
         <v>22</v>
       </c>
-      <c r="H115" s="2">
+      <c r="H115">
         <v>19.3</v>
       </c>
-      <c r="J115" s="2">
+      <c r="J115" s="4">
         <v>44040</v>
       </c>
-      <c r="K115" s="2">
+      <c r="K115" s="4">
         <v>44082</v>
       </c>
       <c r="L115">
@@ -5394,27 +5831,27 @@
         <v>3</v>
       </c>
       <c r="C116" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="D116">
         <v>13</v>
       </c>
-      <c r="E116" s="2">
+      <c r="E116">
         <v>1.81</v>
       </c>
-      <c r="F116" s="2">
+      <c r="F116">
         <v>1.43</v>
       </c>
-      <c r="G116" s="2">
+      <c r="G116">
         <v>18.100000000000001</v>
       </c>
-      <c r="H116" s="2">
+      <c r="H116">
         <v>14.3</v>
       </c>
-      <c r="J116" s="2">
+      <c r="J116" s="4">
         <v>44189</v>
       </c>
-      <c r="K116" s="2">
+      <c r="K116" s="4">
         <v>44238</v>
       </c>
       <c r="L116">
@@ -5431,11 +5868,58 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <conditionalFormatting sqref="A2:D1048576">
+    <cfRule type="expression" dxfId="5" priority="2">
+      <formula>COUNTBLANK(A2) &lt;&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:F1048576">
+    <cfRule type="expression" dxfId="4" priority="3">
+      <formula>SUM(COUNTBLANK(E2), COUNTBLANK(G2))=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G1048576">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>SUM(COUNTBLANK(E2), COUNTBLANK(G2))=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H1048576">
+    <cfRule type="expression" dxfId="2" priority="6">
+      <formula>SUM(COUNTBLANK(E2), COUNTBLANK(G2))=2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2:O1048576">
+    <cfRule type="expression" dxfId="1" priority="7">
+      <formula>COUNTBLANK(J2)=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L2:P1048576">
+    <cfRule type="cellIs" dxfId="0" priority="8" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations disablePrompts="1" count="4">
+    <dataValidation operator="equal" allowBlank="1" showErrorMessage="1" sqref="A2:A1116" xr:uid="{00000000-0002-0000-0100-000000000000}">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation type="date" operator="equal" allowBlank="1" showErrorMessage="1" errorTitle="Must be a valid date" error="That's not a valid date" promptTitle="Must be valid date" prompt="That's not a valid date" sqref="J2:J1116" xr:uid="{00000000-0002-0000-0100-000001000000}">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showErrorMessage="1" errorTitle="Must be a valid date later than Start_date" error="Not a valid date or earlier than Start_date: please correct it" promptTitle="Must be a valid date" sqref="K2:K1116" xr:uid="{00000000-0002-0000-0100-000002000000}">
+      <formula1>K2 &gt;= J2</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Must be an integer greater than or equal to zero" promptTitle="Input valid count" prompt="Must be an integer greater than or equal to zero" sqref="L2:P1048576" xr:uid="{E563A075-588D-4DDD-BBFA-8B48AC8F6536}">
+      <formula1>0</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
YP-CORE_2_scores: corrections to conditional formatting and validation in YPwide2.ods & YPwide2.xlsx (errors wouldn't have had any bad effects.  Created CORE_2_scores app from YP-CORE_2_scores, started conversion from YP-CORE to generic adult CORE: tricky!!  Started adding all t the referential values.
</commit_message>
<xml_diff>
--- a/docs/YP-CORE/YPwide2.xlsx
+++ b/docs/YP-CORE/YPwide2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Current_share\Current_Data\MyR\shiny.psyctc.org\docs\YP-CORE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA2A4662-85B9-4169-B261-35014B332EA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B7175C-FB31-4B59-A50D-103357C5F7FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="13125" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="18975" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -268,7 +268,73 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color rgb="FFCC0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCCC"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFCC0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCCC"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFCC0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCCC"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFCC0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCCC"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFCC0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCCC"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFCC0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCCCC"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" shrinkToFit="0"/>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFCC0000"/>
@@ -709,10 +775,11 @@
   <dimension ref="A1:P116"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1830" ySplit="555" topLeftCell="B1" activePane="bottomRight"/>
+      <pane xSplit="1830" ySplit="510" topLeftCell="B1" activePane="bottomRight"/>
+      <selection activeCell="F2" sqref="F2:F1048576"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K2" sqref="K2"/>
+      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5869,36 +5936,36 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:D1048576">
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="11" priority="2">
       <formula>COUNTBLANK(A2) &lt;&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:F1048576">
-    <cfRule type="expression" dxfId="4" priority="3">
+    <cfRule type="expression" dxfId="10" priority="3">
       <formula>SUM(COUNTBLANK(E2), COUNTBLANK(G2))=2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G1048576">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="9" priority="4">
       <formula>SUM(COUNTBLANK(E2), COUNTBLANK(G2))=2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H1048576">
-    <cfRule type="expression" dxfId="2" priority="6">
-      <formula>SUM(COUNTBLANK(E2), COUNTBLANK(G2))=2</formula>
+    <cfRule type="expression" dxfId="6" priority="6">
+      <formula>SUM(COUNTBLANK(F2), COUNTBLANK(H2))=2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:O1048576">
-    <cfRule type="expression" dxfId="1" priority="7">
+    <cfRule type="expression" dxfId="8" priority="7">
       <formula>COUNTBLANK(J2)=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:P1048576">
-    <cfRule type="cellIs" dxfId="0" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="4">
+  <dataValidations count="8">
     <dataValidation operator="equal" allowBlank="1" showErrorMessage="1" sqref="A2:A1116" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
@@ -5914,6 +5981,18 @@
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Must be an integer greater than or equal to zero" promptTitle="Input valid count" prompt="Must be an integer greater than or equal to zero" sqref="L2:P1048576" xr:uid="{E563A075-588D-4DDD-BBFA-8B48AC8F6536}">
       <formula1>0</formula1>
     </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Out of range value" error="Valid scores are between zero and 4, inclusive" promptTitle="Input a valid score" prompt="Input a valid score or leave blank" sqref="E2:E1048576" xr:uid="{810D52B2-F499-4D18-B5E2-29BDF7CA7D05}">
+      <formula1>"and(e2 ge 0, e2 le 4)"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Out of range value" error="Valid scores are between zero and 4, inclusive" promptTitle="Input a valid score" prompt="Input a valid score or leave blank" sqref="F2:F1048576" xr:uid="{3D1F04DA-5648-4F5D-9B55-1899B59E286E}">
+      <formula1>"and(f2 ge 0, f2 le 4)"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Out of range value" error="Valid scores are between zero and 40, inclusive" promptTitle="Input a valid score" prompt="Input a valid score or leave blank" sqref="G2:G1048576" xr:uid="{3AEEE0E5-E348-4D57-8262-0CBE75D584B8}">
+      <formula1>"and(g2 ge 0, g2 le 40)"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Out of range value" error="Valid scores are between zero and 40, inclusive" promptTitle="Input a valid score" prompt="Input a valid score or leave blank" sqref="H2:H1048576" xr:uid="{24D01BBB-2FF4-4AC5-B145-9F0E8FFDDDDF}">
+      <formula1>"and(h2 ge 0, h2 le 40)"</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>